<commit_message>
update CDR query with final energy use
</commit_message>
<xml_diff>
--- a/gcam/output/ssp24p5tol5/iamc_template_gcam_cdr.xlsx
+++ b/gcam/output/ssp24p5tol5/iamc_template_gcam_cdr.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="660" uniqueCount="60">
   <si>
     <t>Scenario</t>
   </si>
@@ -184,7 +184,16 @@
     <t>Carbon Sequestration|Direct Air Capture|Sorbent</t>
   </si>
   <si>
+    <t>Final Energy|Carbon Management|Direct Air Capture|Solvent</t>
+  </si>
+  <si>
+    <t>Final Energy|Carbon Management|Direct Air Capture|Sorbent</t>
+  </si>
+  <si>
     <t>MtC/yr</t>
+  </si>
+  <si>
+    <t>EJ/yr</t>
   </si>
 </sst>
 </file>
@@ -542,7 +551,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:T65"/>
+  <dimension ref="A1:T129"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -624,7 +633,7 @@
         <v>54</v>
       </c>
       <c r="E2" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="H2">
         <v>4.85644E-06</v>
@@ -680,7 +689,7 @@
         <v>55</v>
       </c>
       <c r="E3" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="H3">
         <v>8.932660000000001E-06</v>
@@ -736,7 +745,7 @@
         <v>54</v>
       </c>
       <c r="E4" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="H4">
         <v>0.00020876417</v>
@@ -792,7 +801,7 @@
         <v>55</v>
       </c>
       <c r="E5" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="H5">
         <v>9.968080000000001E-06</v>
@@ -848,7 +857,7 @@
         <v>54</v>
       </c>
       <c r="E6" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="H6">
         <v>0.00019678705</v>
@@ -904,7 +913,7 @@
         <v>55</v>
       </c>
       <c r="E7" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="H7">
         <v>9.04998E-06</v>
@@ -960,7 +969,7 @@
         <v>54</v>
       </c>
       <c r="E8" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="H8">
         <v>0.000656052</v>
@@ -1016,7 +1025,7 @@
         <v>55</v>
       </c>
       <c r="E9" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="H9">
         <v>3.05429E-05</v>
@@ -1072,7 +1081,7 @@
         <v>54</v>
       </c>
       <c r="E10" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="F10">
         <v>0.00016877479</v>
@@ -1134,7 +1143,7 @@
         <v>55</v>
       </c>
       <c r="E11" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="F11">
         <v>1.00878E-06</v>
@@ -1196,7 +1205,7 @@
         <v>54</v>
       </c>
       <c r="E12" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="F12">
         <v>0.00025284442</v>
@@ -1258,7 +1267,7 @@
         <v>55</v>
       </c>
       <c r="E13" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="F13">
         <v>1.65988E-06</v>
@@ -1320,7 +1329,7 @@
         <v>54</v>
       </c>
       <c r="E14" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="F14">
         <v>0.0003148999</v>
@@ -1382,7 +1391,7 @@
         <v>55</v>
       </c>
       <c r="E15" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="F15">
         <v>2.20544E-06</v>
@@ -1444,7 +1453,7 @@
         <v>54</v>
       </c>
       <c r="E16" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="F16">
         <v>2.5231492E-05</v>
@@ -1506,7 +1515,7 @@
         <v>55</v>
       </c>
       <c r="E17" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="F17">
         <v>1.54929E-07</v>
@@ -1568,7 +1577,7 @@
         <v>54</v>
       </c>
       <c r="E18" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="F18">
         <v>2.50827808E-05</v>
@@ -1630,7 +1639,7 @@
         <v>55</v>
       </c>
       <c r="E19" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="F19">
         <v>7.32982E-08</v>
@@ -1692,7 +1701,7 @@
         <v>54</v>
       </c>
       <c r="E20" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="F20">
         <v>0.0002464695</v>
@@ -1754,7 +1763,7 @@
         <v>55</v>
       </c>
       <c r="E21" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="F21">
         <v>9.582720000000001E-07</v>
@@ -1816,7 +1825,7 @@
         <v>54</v>
       </c>
       <c r="E22" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="H22">
         <v>0.016851772</v>
@@ -1872,7 +1881,7 @@
         <v>55</v>
       </c>
       <c r="E23" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="H23">
         <v>0.00169432</v>
@@ -1928,7 +1937,7 @@
         <v>54</v>
       </c>
       <c r="E24" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="F24">
         <v>6.882594299999999E-05</v>
@@ -1990,7 +1999,7 @@
         <v>55</v>
       </c>
       <c r="E25" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="F25">
         <v>4.16576E-07</v>
@@ -2052,7 +2061,7 @@
         <v>54</v>
       </c>
       <c r="E26" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="F26">
         <v>7.2946447E-06</v>
@@ -2114,7 +2123,7 @@
         <v>55</v>
       </c>
       <c r="E27" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="F27">
         <v>3.18926E-08</v>
@@ -2176,7 +2185,7 @@
         <v>54</v>
       </c>
       <c r="E28" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="F28">
         <v>1.8732708E-05</v>
@@ -2238,7 +2247,7 @@
         <v>55</v>
       </c>
       <c r="E29" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="F29">
         <v>1.15776E-07</v>
@@ -2300,7 +2309,7 @@
         <v>54</v>
       </c>
       <c r="E30" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="H30">
         <v>0.00019134984</v>
@@ -2356,7 +2365,7 @@
         <v>55</v>
       </c>
       <c r="E31" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="H31">
         <v>1.08525E-05</v>
@@ -2412,7 +2421,7 @@
         <v>54</v>
       </c>
       <c r="E32" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="F32">
         <v>2.6809138E-06</v>
@@ -2474,7 +2483,7 @@
         <v>55</v>
       </c>
       <c r="E33" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="F33">
         <v>2.64319E-08</v>
@@ -2536,7 +2545,7 @@
         <v>54</v>
       </c>
       <c r="E34" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="F34">
         <v>8.344701399999999E-06</v>
@@ -2598,7 +2607,7 @@
         <v>55</v>
       </c>
       <c r="E35" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="F35">
         <v>4.85667E-08</v>
@@ -2660,7 +2669,7 @@
         <v>54</v>
       </c>
       <c r="E36" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="F36">
         <v>3.914865499999999E-06</v>
@@ -2722,7 +2731,7 @@
         <v>55</v>
       </c>
       <c r="E37" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="F37">
         <v>1.36434E-08</v>
@@ -2784,7 +2793,7 @@
         <v>54</v>
       </c>
       <c r="E38" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="F38">
         <v>1.2821307E-05</v>
@@ -2846,7 +2855,7 @@
         <v>55</v>
       </c>
       <c r="E39" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="F39">
         <v>9.78425E-08</v>
@@ -2908,7 +2917,7 @@
         <v>54</v>
       </c>
       <c r="E40" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="F40">
         <v>0.0001289417</v>
@@ -2970,7 +2979,7 @@
         <v>55</v>
       </c>
       <c r="E41" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="F41">
         <v>7.64824E-07</v>
@@ -3032,7 +3041,7 @@
         <v>54</v>
       </c>
       <c r="E42" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="F42">
         <v>0.000128242202</v>
@@ -3094,7 +3103,7 @@
         <v>55</v>
       </c>
       <c r="E43" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="F43">
         <v>5.350609999999999E-07</v>
@@ -3156,7 +3165,7 @@
         <v>54</v>
       </c>
       <c r="E44" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="H44">
         <v>2.8694078E-05</v>
@@ -3212,7 +3221,7 @@
         <v>55</v>
       </c>
       <c r="E45" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="H45">
         <v>2.03657E-06</v>
@@ -3268,7 +3277,7 @@
         <v>54</v>
       </c>
       <c r="E46" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="H46">
         <v>0.0047368213</v>
@@ -3324,7 +3333,7 @@
         <v>55</v>
       </c>
       <c r="E47" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="H47">
         <v>0.000187604</v>
@@ -3380,7 +3389,7 @@
         <v>54</v>
       </c>
       <c r="E48" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="F48">
         <v>1.333818E-06</v>
@@ -3442,7 +3451,7 @@
         <v>55</v>
       </c>
       <c r="E49" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="F49">
         <v>1.84157E-08</v>
@@ -3504,7 +3513,7 @@
         <v>54</v>
       </c>
       <c r="E50" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="F50">
         <v>3.82362955E-05</v>
@@ -3566,7 +3575,7 @@
         <v>55</v>
       </c>
       <c r="E51" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="F51">
         <v>5.9494E-08</v>
@@ -3628,7 +3637,7 @@
         <v>54</v>
       </c>
       <c r="E52" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="F52">
         <v>0.00019293616</v>
@@ -3690,7 +3699,7 @@
         <v>55</v>
       </c>
       <c r="E53" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="F53">
         <v>1.21604E-06</v>
@@ -3752,7 +3761,7 @@
         <v>54</v>
       </c>
       <c r="E54" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="H54">
         <v>2.1193322E-05</v>
@@ -3808,7 +3817,7 @@
         <v>55</v>
       </c>
       <c r="E55" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="H55">
         <v>2.23747E-06</v>
@@ -3864,7 +3873,7 @@
         <v>54</v>
       </c>
       <c r="E56" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="H56">
         <v>0.0016856193</v>
@@ -3920,7 +3929,7 @@
         <v>55</v>
       </c>
       <c r="E57" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="H57">
         <v>0.000120426</v>
@@ -3976,7 +3985,7 @@
         <v>54</v>
       </c>
       <c r="E58" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="F58">
         <v>5.1571845E-08</v>
@@ -4020,7 +4029,7 @@
         <v>55</v>
       </c>
       <c r="E59" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="F59">
         <v>5.14823E-10</v>
@@ -4064,7 +4073,7 @@
         <v>54</v>
       </c>
       <c r="E60" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="F60">
         <v>0.0010135465</v>
@@ -4126,7 +4135,7 @@
         <v>55</v>
       </c>
       <c r="E61" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="F61">
         <v>6.33177E-06</v>
@@ -4188,7 +4197,7 @@
         <v>54</v>
       </c>
       <c r="E62" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="H62">
         <v>9.803223900000001E-05</v>
@@ -4244,7 +4253,7 @@
         <v>55</v>
       </c>
       <c r="E63" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="H63">
         <v>3.05205E-06</v>
@@ -4300,7 +4309,7 @@
         <v>54</v>
       </c>
       <c r="E64" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="F64">
         <v>0.002659206213545</v>
@@ -4362,7 +4371,7 @@
         <v>55</v>
       </c>
       <c r="E65" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="F65">
         <v>1.5737447823E-05</v>
@@ -4408,6 +4417,3800 @@
       </c>
       <c r="T65">
         <v>257.5691281749202</v>
+      </c>
+    </row>
+    <row r="66" spans="1:20">
+      <c r="A66" t="s">
+        <v>20</v>
+      </c>
+      <c r="B66" t="s">
+        <v>21</v>
+      </c>
+      <c r="C66" t="s">
+        <v>53</v>
+      </c>
+      <c r="D66" t="s">
+        <v>56</v>
+      </c>
+      <c r="E66" t="s">
+        <v>59</v>
+      </c>
+      <c r="H66">
+        <v>6.54231E-08</v>
+      </c>
+      <c r="I66">
+        <v>5.96937E-07</v>
+      </c>
+      <c r="J66">
+        <v>6.81027E-06</v>
+      </c>
+      <c r="K66">
+        <v>9.45965E-06</v>
+      </c>
+      <c r="L66">
+        <v>1.293659E-05</v>
+      </c>
+      <c r="M66">
+        <v>1.74027E-05</v>
+      </c>
+      <c r="N66">
+        <v>1.959949E-05</v>
+      </c>
+      <c r="O66">
+        <v>1.763035E-05</v>
+      </c>
+      <c r="P66">
+        <v>1.437106E-05</v>
+      </c>
+      <c r="Q66">
+        <v>5.934667000000001E-06</v>
+      </c>
+      <c r="R66">
+        <v>2.679356E-06</v>
+      </c>
+      <c r="S66">
+        <v>1.33614E-06</v>
+      </c>
+      <c r="T66">
+        <v>1.452137E-06</v>
+      </c>
+    </row>
+    <row r="67" spans="1:20">
+      <c r="A67" t="s">
+        <v>20</v>
+      </c>
+      <c r="B67" t="s">
+        <v>21</v>
+      </c>
+      <c r="C67" t="s">
+        <v>53</v>
+      </c>
+      <c r="D67" t="s">
+        <v>57</v>
+      </c>
+      <c r="E67" t="s">
+        <v>59</v>
+      </c>
+      <c r="H67">
+        <v>1.21658E-07</v>
+      </c>
+      <c r="I67">
+        <v>1.9362E-06</v>
+      </c>
+      <c r="J67">
+        <v>3.73986E-05</v>
+      </c>
+      <c r="K67">
+        <v>5.11754E-05</v>
+      </c>
+      <c r="L67">
+        <v>7.031130000000001E-05</v>
+      </c>
+      <c r="M67">
+        <v>9.60836E-05</v>
+      </c>
+      <c r="N67">
+        <v>0.000110674126313</v>
+      </c>
+      <c r="O67">
+        <v>0.000102302</v>
+      </c>
+      <c r="P67">
+        <v>8.77336E-05</v>
+      </c>
+      <c r="Q67">
+        <v>3.75026E-05</v>
+      </c>
+      <c r="R67">
+        <v>1.72843E-05</v>
+      </c>
+      <c r="S67">
+        <v>8.612719999999999E-06</v>
+      </c>
+      <c r="T67">
+        <v>4.76083E-06</v>
+      </c>
+    </row>
+    <row r="68" spans="1:20">
+      <c r="A68" t="s">
+        <v>20</v>
+      </c>
+      <c r="B68" t="s">
+        <v>22</v>
+      </c>
+      <c r="C68" t="s">
+        <v>53</v>
+      </c>
+      <c r="D68" t="s">
+        <v>56</v>
+      </c>
+      <c r="E68" t="s">
+        <v>59</v>
+      </c>
+      <c r="H68">
+        <v>1.1935095E-06</v>
+      </c>
+      <c r="I68">
+        <v>7.368103E-06</v>
+      </c>
+      <c r="J68">
+        <v>4.449208E-05</v>
+      </c>
+      <c r="K68">
+        <v>4.828109E-05</v>
+      </c>
+      <c r="L68">
+        <v>5.255541E-05</v>
+      </c>
+      <c r="M68">
+        <v>3.683762E-05</v>
+      </c>
+      <c r="N68">
+        <v>2.583087E-05</v>
+      </c>
+      <c r="O68">
+        <v>1.912754E-05</v>
+      </c>
+      <c r="P68">
+        <v>1.421023E-05</v>
+      </c>
+      <c r="Q68">
+        <v>5.873469999999999E-06</v>
+      </c>
+      <c r="R68">
+        <v>2.737311E-06</v>
+      </c>
+      <c r="S68">
+        <v>1.424217E-06</v>
+      </c>
+      <c r="T68">
+        <v>8.16381E-07</v>
+      </c>
+    </row>
+    <row r="69" spans="1:20">
+      <c r="A69" t="s">
+        <v>20</v>
+      </c>
+      <c r="B69" t="s">
+        <v>22</v>
+      </c>
+      <c r="C69" t="s">
+        <v>53</v>
+      </c>
+      <c r="D69" t="s">
+        <v>57</v>
+      </c>
+      <c r="E69" t="s">
+        <v>59</v>
+      </c>
+      <c r="H69">
+        <v>1.3576E-07</v>
+      </c>
+      <c r="I69">
+        <v>2.24575E-06</v>
+      </c>
+      <c r="J69">
+        <v>3.68467E-05</v>
+      </c>
+      <c r="K69">
+        <v>4.35328E-05</v>
+      </c>
+      <c r="L69">
+        <v>5.16256E-05</v>
+      </c>
+      <c r="M69">
+        <v>4.26238E-05</v>
+      </c>
+      <c r="N69">
+        <v>3.56628E-05</v>
+      </c>
+      <c r="O69">
+        <v>3.1954E-05</v>
+      </c>
+      <c r="P69">
+        <v>2.90422E-05</v>
+      </c>
+      <c r="Q69">
+        <v>1.43619E-05</v>
+      </c>
+      <c r="R69">
+        <v>7.71169E-06</v>
+      </c>
+      <c r="S69">
+        <v>4.45324E-06</v>
+      </c>
+      <c r="T69">
+        <v>2.79402E-06</v>
+      </c>
+    </row>
+    <row r="70" spans="1:20">
+      <c r="A70" t="s">
+        <v>20</v>
+      </c>
+      <c r="B70" t="s">
+        <v>23</v>
+      </c>
+      <c r="C70" t="s">
+        <v>53</v>
+      </c>
+      <c r="D70" t="s">
+        <v>56</v>
+      </c>
+      <c r="E70" t="s">
+        <v>59</v>
+      </c>
+      <c r="H70">
+        <v>1.118587E-06</v>
+      </c>
+      <c r="I70">
+        <v>5.001236E-06</v>
+      </c>
+      <c r="J70">
+        <v>3.404089E-05</v>
+      </c>
+      <c r="K70">
+        <v>4.150439E-05</v>
+      </c>
+      <c r="L70">
+        <v>4.833084E-05</v>
+      </c>
+      <c r="M70">
+        <v>5.586665E-05</v>
+      </c>
+      <c r="N70">
+        <v>4.367203E-05</v>
+      </c>
+      <c r="O70">
+        <v>3.052736E-05</v>
+      </c>
+      <c r="P70">
+        <v>2.019063E-05</v>
+      </c>
+      <c r="Q70">
+        <v>7.180559999999999E-06</v>
+      </c>
+      <c r="R70">
+        <v>2.892482E-06</v>
+      </c>
+      <c r="S70">
+        <v>1.333883E-06</v>
+      </c>
+      <c r="T70">
+        <v>6.71296E-07</v>
+      </c>
+    </row>
+    <row r="71" spans="1:20">
+      <c r="A71" t="s">
+        <v>20</v>
+      </c>
+      <c r="B71" t="s">
+        <v>23</v>
+      </c>
+      <c r="C71" t="s">
+        <v>53</v>
+      </c>
+      <c r="D71" t="s">
+        <v>57</v>
+      </c>
+      <c r="E71" t="s">
+        <v>59</v>
+      </c>
+      <c r="H71">
+        <v>1.23256E-07</v>
+      </c>
+      <c r="I71">
+        <v>1.73909E-06</v>
+      </c>
+      <c r="J71">
+        <v>3.23465E-05</v>
+      </c>
+      <c r="K71">
+        <v>4.13716E-05</v>
+      </c>
+      <c r="L71">
+        <v>5.28417E-05</v>
+      </c>
+      <c r="M71">
+        <v>6.65687E-05</v>
+      </c>
+      <c r="N71">
+        <v>6.05283E-05</v>
+      </c>
+      <c r="O71">
+        <v>5.12891E-05</v>
+      </c>
+      <c r="P71">
+        <v>4.16595E-05</v>
+      </c>
+      <c r="Q71">
+        <v>1.79016E-05</v>
+      </c>
+      <c r="R71">
+        <v>8.407260000000001E-06</v>
+      </c>
+      <c r="S71">
+        <v>4.33735E-06</v>
+      </c>
+      <c r="T71">
+        <v>2.38071E-06</v>
+      </c>
+    </row>
+    <row r="72" spans="1:20">
+      <c r="A72" t="s">
+        <v>20</v>
+      </c>
+      <c r="B72" t="s">
+        <v>24</v>
+      </c>
+      <c r="C72" t="s">
+        <v>53</v>
+      </c>
+      <c r="D72" t="s">
+        <v>56</v>
+      </c>
+      <c r="E72" t="s">
+        <v>59</v>
+      </c>
+      <c r="H72">
+        <v>3.762659E-06</v>
+      </c>
+      <c r="I72">
+        <v>1.806816E-05</v>
+      </c>
+      <c r="J72">
+        <v>0.0001074933</v>
+      </c>
+      <c r="K72">
+        <v>0.0001311945</v>
+      </c>
+      <c r="L72">
+        <v>0.0001611939</v>
+      </c>
+      <c r="M72">
+        <v>0.0002050938</v>
+      </c>
+      <c r="N72">
+        <v>0.0002590481</v>
+      </c>
+      <c r="O72">
+        <v>0.0002073112</v>
+      </c>
+      <c r="P72">
+        <v>0.0001393735</v>
+      </c>
+      <c r="Q72">
+        <v>4.36352E-05</v>
+      </c>
+      <c r="R72">
+        <v>1.441187E-05</v>
+      </c>
+      <c r="S72">
+        <v>5.31564E-06</v>
+      </c>
+      <c r="T72">
+        <v>2.267394E-06</v>
+      </c>
+    </row>
+    <row r="73" spans="1:20">
+      <c r="A73" t="s">
+        <v>20</v>
+      </c>
+      <c r="B73" t="s">
+        <v>24</v>
+      </c>
+      <c r="C73" t="s">
+        <v>53</v>
+      </c>
+      <c r="D73" t="s">
+        <v>57</v>
+      </c>
+      <c r="E73" t="s">
+        <v>59</v>
+      </c>
+      <c r="H73">
+        <v>4.15979E-07</v>
+      </c>
+      <c r="I73">
+        <v>5.80909E-06</v>
+      </c>
+      <c r="J73">
+        <v>9.222210000000001E-05</v>
+      </c>
+      <c r="K73">
+        <v>0.000119917</v>
+      </c>
+      <c r="L73">
+        <v>0.000158286</v>
+      </c>
+      <c r="M73">
+        <v>0.000213227805062</v>
+      </c>
+      <c r="N73">
+        <v>0.00029214956</v>
+      </c>
+      <c r="O73">
+        <v>0.0002748691754</v>
+      </c>
+      <c r="P73">
+        <v>0.000228357176929</v>
+      </c>
+      <c r="Q73">
+        <v>9.01563E-05</v>
+      </c>
+      <c r="R73">
+        <v>3.65091E-05</v>
+      </c>
+      <c r="S73">
+        <v>1.58752E-05</v>
+      </c>
+      <c r="T73">
+        <v>7.675739999999999E-06</v>
+      </c>
+    </row>
+    <row r="74" spans="1:20">
+      <c r="A74" t="s">
+        <v>20</v>
+      </c>
+      <c r="B74" t="s">
+        <v>25</v>
+      </c>
+      <c r="C74" t="s">
+        <v>53</v>
+      </c>
+      <c r="D74" t="s">
+        <v>56</v>
+      </c>
+      <c r="E74" t="s">
+        <v>59</v>
+      </c>
+      <c r="F74">
+        <v>1.064215E-06</v>
+      </c>
+      <c r="G74">
+        <v>4.948371000000001E-06</v>
+      </c>
+      <c r="H74">
+        <v>3.39228E-05</v>
+      </c>
+      <c r="I74">
+        <v>0.0002669573</v>
+      </c>
+      <c r="J74">
+        <v>0.001829423</v>
+      </c>
+      <c r="K74">
+        <v>0.0023354782918</v>
+      </c>
+      <c r="L74">
+        <v>0.00507451242878</v>
+      </c>
+      <c r="M74">
+        <v>0.01016541835031</v>
+      </c>
+      <c r="N74">
+        <v>0.01521028656291</v>
+      </c>
+      <c r="O74">
+        <v>0.025328497694715</v>
+      </c>
+      <c r="P74">
+        <v>0.0462961024746089</v>
+      </c>
+      <c r="Q74">
+        <v>0.068780779946349</v>
+      </c>
+      <c r="R74">
+        <v>0.095788868242493</v>
+      </c>
+      <c r="S74">
+        <v>0.115558728516702</v>
+      </c>
+      <c r="T74">
+        <v>0.133123242389127</v>
+      </c>
+    </row>
+    <row r="75" spans="1:20">
+      <c r="A75" t="s">
+        <v>20</v>
+      </c>
+      <c r="B75" t="s">
+        <v>25</v>
+      </c>
+      <c r="C75" t="s">
+        <v>53</v>
+      </c>
+      <c r="D75" t="s">
+        <v>57</v>
+      </c>
+      <c r="E75" t="s">
+        <v>59</v>
+      </c>
+      <c r="F75">
+        <v>1.80762E-08</v>
+      </c>
+      <c r="G75">
+        <v>2.48757E-07</v>
+      </c>
+      <c r="H75">
+        <v>4.35888E-06</v>
+      </c>
+      <c r="I75">
+        <v>8.474139999999999E-05</v>
+      </c>
+      <c r="J75">
+        <v>0.00146301</v>
+      </c>
+      <c r="K75">
+        <v>0.002727881</v>
+      </c>
+      <c r="L75">
+        <v>0.006061991947</v>
+      </c>
+      <c r="M75">
+        <v>0.009832200100000001</v>
+      </c>
+      <c r="N75">
+        <v>0.01528772370139</v>
+      </c>
+      <c r="O75">
+        <v>0.02635303836685</v>
+      </c>
+      <c r="P75">
+        <v>0.05036722950824</v>
+      </c>
+      <c r="Q75">
+        <v>0.07370950848153</v>
+      </c>
+      <c r="R75">
+        <v>0.0954750670641</v>
+      </c>
+      <c r="S75">
+        <v>0.114218039912</v>
+      </c>
+      <c r="T75">
+        <v>0.12958736695</v>
+      </c>
+    </row>
+    <row r="76" spans="1:20">
+      <c r="A76" t="s">
+        <v>20</v>
+      </c>
+      <c r="B76" t="s">
+        <v>26</v>
+      </c>
+      <c r="C76" t="s">
+        <v>53</v>
+      </c>
+      <c r="D76" t="s">
+        <v>56</v>
+      </c>
+      <c r="E76" t="s">
+        <v>59</v>
+      </c>
+      <c r="F76">
+        <v>1.5986983E-06</v>
+      </c>
+      <c r="G76">
+        <v>7.489636E-06</v>
+      </c>
+      <c r="H76">
+        <v>3.096079E-05</v>
+      </c>
+      <c r="I76">
+        <v>0.0002319315</v>
+      </c>
+      <c r="J76">
+        <v>0.001569278</v>
+      </c>
+      <c r="K76">
+        <v>0.002075461131342</v>
+      </c>
+      <c r="L76">
+        <v>0.00261479318095</v>
+      </c>
+      <c r="M76">
+        <v>0.003646184265164</v>
+      </c>
+      <c r="N76">
+        <v>0.0139707206924</v>
+      </c>
+      <c r="O76">
+        <v>0.025687385432986</v>
+      </c>
+      <c r="P76">
+        <v>0.054294087543607</v>
+      </c>
+      <c r="Q76">
+        <v>0.08504230960228</v>
+      </c>
+      <c r="R76">
+        <v>0.11557819070937</v>
+      </c>
+      <c r="S76">
+        <v>0.140545344618805</v>
+      </c>
+      <c r="T76">
+        <v>0.163716536269092</v>
+      </c>
+    </row>
+    <row r="77" spans="1:20">
+      <c r="A77" t="s">
+        <v>20</v>
+      </c>
+      <c r="B77" t="s">
+        <v>26</v>
+      </c>
+      <c r="C77" t="s">
+        <v>53</v>
+      </c>
+      <c r="D77" t="s">
+        <v>57</v>
+      </c>
+      <c r="E77" t="s">
+        <v>59</v>
+      </c>
+      <c r="F77">
+        <v>2.97431E-08</v>
+      </c>
+      <c r="G77">
+        <v>4.72809E-07</v>
+      </c>
+      <c r="H77">
+        <v>5.54522E-06</v>
+      </c>
+      <c r="I77">
+        <v>9.97233E-05</v>
+      </c>
+      <c r="J77">
+        <v>0.00163934</v>
+      </c>
+      <c r="K77">
+        <v>0.002112474488</v>
+      </c>
+      <c r="L77">
+        <v>0.0063509599999999</v>
+      </c>
+      <c r="M77">
+        <v>0.0100133611069</v>
+      </c>
+      <c r="N77">
+        <v>0.016902659534</v>
+      </c>
+      <c r="O77">
+        <v>0.0311948272084</v>
+      </c>
+      <c r="P77">
+        <v>0.0624618257764899</v>
+      </c>
+      <c r="Q77">
+        <v>0.09201586512299</v>
+      </c>
+      <c r="R77">
+        <v>0.1190083265348</v>
+      </c>
+      <c r="S77">
+        <v>0.141763146567</v>
+      </c>
+      <c r="T77">
+        <v>0.15998579601</v>
+      </c>
+    </row>
+    <row r="78" spans="1:20">
+      <c r="A78" t="s">
+        <v>20</v>
+      </c>
+      <c r="B78" t="s">
+        <v>27</v>
+      </c>
+      <c r="C78" t="s">
+        <v>53</v>
+      </c>
+      <c r="D78" t="s">
+        <v>56</v>
+      </c>
+      <c r="E78" t="s">
+        <v>59</v>
+      </c>
+      <c r="F78">
+        <v>1.9921398E-06</v>
+      </c>
+      <c r="G78">
+        <v>8.973855999999999E-06</v>
+      </c>
+      <c r="H78">
+        <v>5.815748E-05</v>
+      </c>
+      <c r="I78">
+        <v>0.0004187383</v>
+      </c>
+      <c r="J78">
+        <v>0.002921984</v>
+      </c>
+      <c r="K78">
+        <v>0.003501305</v>
+      </c>
+      <c r="L78">
+        <v>0.00447702</v>
+      </c>
+      <c r="M78">
+        <v>0.0058849322753559</v>
+      </c>
+      <c r="N78">
+        <v>0.01016787037718</v>
+      </c>
+      <c r="O78">
+        <v>0.0389723562236059</v>
+      </c>
+      <c r="P78">
+        <v>0.07856311562569999</v>
+      </c>
+      <c r="Q78">
+        <v>0.11188216275824</v>
+      </c>
+      <c r="R78">
+        <v>0.1440586291418</v>
+      </c>
+      <c r="S78">
+        <v>0.17371086133731</v>
+      </c>
+      <c r="T78">
+        <v>0.20259540663486</v>
+      </c>
+    </row>
+    <row r="79" spans="1:20">
+      <c r="A79" t="s">
+        <v>20</v>
+      </c>
+      <c r="B79" t="s">
+        <v>27</v>
+      </c>
+      <c r="C79" t="s">
+        <v>53</v>
+      </c>
+      <c r="D79" t="s">
+        <v>57</v>
+      </c>
+      <c r="E79" t="s">
+        <v>59</v>
+      </c>
+      <c r="F79">
+        <v>3.95188E-08</v>
+      </c>
+      <c r="G79">
+        <v>5.58118E-07</v>
+      </c>
+      <c r="H79">
+        <v>1.06752E-05</v>
+      </c>
+      <c r="I79">
+        <v>0.000207994</v>
+      </c>
+      <c r="J79">
+        <v>0.00368674</v>
+      </c>
+      <c r="K79">
+        <v>0.0047574671894</v>
+      </c>
+      <c r="L79">
+        <v>0.01435012</v>
+      </c>
+      <c r="M79">
+        <v>0.02246677207703</v>
+      </c>
+      <c r="N79">
+        <v>0.03658464</v>
+      </c>
+      <c r="O79">
+        <v>0.06596031553999999</v>
+      </c>
+      <c r="P79">
+        <v>0.131098445118</v>
+      </c>
+      <c r="Q79">
+        <v>0.194267119074135</v>
+      </c>
+      <c r="R79">
+        <v>0.2529585085435</v>
+      </c>
+      <c r="S79">
+        <v>0.303977539314</v>
+      </c>
+      <c r="T79">
+        <v>0.3469141956</v>
+      </c>
+    </row>
+    <row r="80" spans="1:20">
+      <c r="A80" t="s">
+        <v>20</v>
+      </c>
+      <c r="B80" t="s">
+        <v>28</v>
+      </c>
+      <c r="C80" t="s">
+        <v>53</v>
+      </c>
+      <c r="D80" t="s">
+        <v>56</v>
+      </c>
+      <c r="E80" t="s">
+        <v>59</v>
+      </c>
+      <c r="F80">
+        <v>1.5885548E-07</v>
+      </c>
+      <c r="G80">
+        <v>9.535061E-07</v>
+      </c>
+      <c r="H80">
+        <v>4.338474E-06</v>
+      </c>
+      <c r="I80">
+        <v>2.796867E-05</v>
+      </c>
+      <c r="J80">
+        <v>0.000154894</v>
+      </c>
+      <c r="K80">
+        <v>0.0002154635</v>
+      </c>
+      <c r="L80">
+        <v>0.000330283</v>
+      </c>
+      <c r="M80">
+        <v>0.000545966535676</v>
+      </c>
+      <c r="N80">
+        <v>0.001759476261823</v>
+      </c>
+      <c r="O80">
+        <v>0.0031558281645</v>
+      </c>
+      <c r="P80">
+        <v>0.0057337741190979</v>
+      </c>
+      <c r="Q80">
+        <v>0.007468557183099999</v>
+      </c>
+      <c r="R80">
+        <v>0.0089525861398099</v>
+      </c>
+      <c r="S80">
+        <v>0.010052251612941</v>
+      </c>
+      <c r="T80">
+        <v>0.010514631805059</v>
+      </c>
+    </row>
+    <row r="81" spans="1:20">
+      <c r="A81" t="s">
+        <v>20</v>
+      </c>
+      <c r="B81" t="s">
+        <v>28</v>
+      </c>
+      <c r="C81" t="s">
+        <v>53</v>
+      </c>
+      <c r="D81" t="s">
+        <v>57</v>
+      </c>
+      <c r="E81" t="s">
+        <v>59</v>
+      </c>
+      <c r="F81">
+        <v>2.77615E-09</v>
+      </c>
+      <c r="G81">
+        <v>4.92057E-08</v>
+      </c>
+      <c r="H81">
+        <v>6.45991E-07</v>
+      </c>
+      <c r="I81">
+        <v>1.20792E-05</v>
+      </c>
+      <c r="J81">
+        <v>0.000188374</v>
+      </c>
+      <c r="K81">
+        <v>0.000283353</v>
+      </c>
+      <c r="L81">
+        <v>0.000441348177</v>
+      </c>
+      <c r="M81">
+        <v>0.001559864562849</v>
+      </c>
+      <c r="N81">
+        <v>0.00275155398</v>
+      </c>
+      <c r="O81">
+        <v>0.005072540724</v>
+      </c>
+      <c r="P81">
+        <v>0.00974497879299</v>
+      </c>
+      <c r="Q81">
+        <v>0.01391130670467</v>
+      </c>
+      <c r="R81">
+        <v>0.01737327656819</v>
+      </c>
+      <c r="S81">
+        <v>0.0198624209282999</v>
+      </c>
+      <c r="T81">
+        <v>0.020988955506</v>
+      </c>
+    </row>
+    <row r="82" spans="1:20">
+      <c r="A82" t="s">
+        <v>20</v>
+      </c>
+      <c r="B82" t="s">
+        <v>29</v>
+      </c>
+      <c r="C82" t="s">
+        <v>53</v>
+      </c>
+      <c r="D82" t="s">
+        <v>56</v>
+      </c>
+      <c r="E82" t="s">
+        <v>59</v>
+      </c>
+      <c r="F82">
+        <v>1.5616348E-07</v>
+      </c>
+      <c r="G82">
+        <v>7.199053E-07</v>
+      </c>
+      <c r="H82">
+        <v>4.612644E-06</v>
+      </c>
+      <c r="I82">
+        <v>3.084022E-05</v>
+      </c>
+      <c r="J82">
+        <v>0.000163195</v>
+      </c>
+      <c r="K82">
+        <v>0.0002143262</v>
+      </c>
+      <c r="L82">
+        <v>0.000325675</v>
+      </c>
+      <c r="M82">
+        <v>0.0005155642887889</v>
+      </c>
+      <c r="N82">
+        <v>0.0019001671167</v>
+      </c>
+      <c r="O82">
+        <v>0.003388848834025</v>
+      </c>
+      <c r="P82">
+        <v>0.0061214814344</v>
+      </c>
+      <c r="Q82">
+        <v>0.0082291054552</v>
+      </c>
+      <c r="R82">
+        <v>0.009979817864558999</v>
+      </c>
+      <c r="S82">
+        <v>0.0111500711787</v>
+      </c>
+      <c r="T82">
+        <v>0.01163973320218</v>
+      </c>
+    </row>
+    <row r="83" spans="1:20">
+      <c r="A83" t="s">
+        <v>20</v>
+      </c>
+      <c r="B83" t="s">
+        <v>29</v>
+      </c>
+      <c r="C83" t="s">
+        <v>53</v>
+      </c>
+      <c r="D83" t="s">
+        <v>57</v>
+      </c>
+      <c r="E83" t="s">
+        <v>59</v>
+      </c>
+      <c r="F83">
+        <v>1.31342E-09</v>
+      </c>
+      <c r="G83">
+        <v>1.97932E-08</v>
+      </c>
+      <c r="H83">
+        <v>3.85921E-07</v>
+      </c>
+      <c r="I83">
+        <v>7.79177E-06</v>
+      </c>
+      <c r="J83">
+        <v>0.000125859</v>
+      </c>
+      <c r="K83">
+        <v>0.000178498</v>
+      </c>
+      <c r="L83">
+        <v>0.000282515</v>
+      </c>
+      <c r="M83">
+        <v>0.000465654804</v>
+      </c>
+      <c r="N83">
+        <v>0.001776897304798</v>
+      </c>
+      <c r="O83">
+        <v>0.00332539026</v>
+      </c>
+      <c r="P83">
+        <v>0.006417467946</v>
+      </c>
+      <c r="Q83">
+        <v>0.0091811750015</v>
+      </c>
+      <c r="R83">
+        <v>0.0115082117497</v>
+      </c>
+      <c r="S83">
+        <v>0.0130963643071</v>
+      </c>
+      <c r="T83">
+        <v>0.013760460757</v>
+      </c>
+    </row>
+    <row r="84" spans="1:20">
+      <c r="A84" t="s">
+        <v>20</v>
+      </c>
+      <c r="B84" t="s">
+        <v>30</v>
+      </c>
+      <c r="C84" t="s">
+        <v>53</v>
+      </c>
+      <c r="D84" t="s">
+        <v>56</v>
+      </c>
+      <c r="E84" t="s">
+        <v>59</v>
+      </c>
+      <c r="F84">
+        <v>1.5406274E-06</v>
+      </c>
+      <c r="G84">
+        <v>8.373830999999999E-06</v>
+      </c>
+      <c r="H84">
+        <v>3.571653E-05</v>
+      </c>
+      <c r="I84">
+        <v>0.0002638402</v>
+      </c>
+      <c r="J84">
+        <v>0.001681591</v>
+      </c>
+      <c r="K84">
+        <v>0.002061583273729</v>
+      </c>
+      <c r="L84">
+        <v>0.00240407100207</v>
+      </c>
+      <c r="M84">
+        <v>0.0036754597259499</v>
+      </c>
+      <c r="N84">
+        <v>0.0142163573203</v>
+      </c>
+      <c r="O84">
+        <v>0.0250053195189999</v>
+      </c>
+      <c r="P84">
+        <v>0.04633388103387</v>
+      </c>
+      <c r="Q84">
+        <v>0.06394644789911</v>
+      </c>
+      <c r="R84">
+        <v>0.07921626881252</v>
+      </c>
+      <c r="S84">
+        <v>0.09154561362822</v>
+      </c>
+      <c r="T84">
+        <v>0.101364289699332</v>
+      </c>
+    </row>
+    <row r="85" spans="1:20">
+      <c r="A85" t="s">
+        <v>20</v>
+      </c>
+      <c r="B85" t="s">
+        <v>30</v>
+      </c>
+      <c r="C85" t="s">
+        <v>53</v>
+      </c>
+      <c r="D85" t="s">
+        <v>57</v>
+      </c>
+      <c r="E85" t="s">
+        <v>59</v>
+      </c>
+      <c r="F85">
+        <v>1.71711E-08</v>
+      </c>
+      <c r="G85">
+        <v>2.88716E-07</v>
+      </c>
+      <c r="H85">
+        <v>3.77398E-06</v>
+      </c>
+      <c r="I85">
+        <v>7.407009999999999E-05</v>
+      </c>
+      <c r="J85">
+        <v>0.00124881</v>
+      </c>
+      <c r="K85">
+        <v>0.001603990890475</v>
+      </c>
+      <c r="L85">
+        <v>0.0020542444212</v>
+      </c>
+      <c r="M85">
+        <v>0.007834820160914999</v>
+      </c>
+      <c r="N85">
+        <v>0.01346535</v>
+      </c>
+      <c r="O85">
+        <v>0.02503639533</v>
+      </c>
+      <c r="P85">
+        <v>0.0492420999033</v>
+      </c>
+      <c r="Q85">
+        <v>0.07221325786210001</v>
+      </c>
+      <c r="R85">
+        <v>0.0928841741268</v>
+      </c>
+      <c r="S85">
+        <v>0.11006501188</v>
+      </c>
+      <c r="T85">
+        <v>0.12355779012</v>
+      </c>
+    </row>
+    <row r="86" spans="1:20">
+      <c r="A86" t="s">
+        <v>20</v>
+      </c>
+      <c r="B86" t="s">
+        <v>31</v>
+      </c>
+      <c r="C86" t="s">
+        <v>53</v>
+      </c>
+      <c r="D86" t="s">
+        <v>56</v>
+      </c>
+      <c r="E86" t="s">
+        <v>59</v>
+      </c>
+      <c r="H86">
+        <v>0.000103014</v>
+      </c>
+      <c r="I86">
+        <v>0.000561544</v>
+      </c>
+      <c r="J86">
+        <v>0.003017425</v>
+      </c>
+      <c r="K86">
+        <v>0.00418666</v>
+      </c>
+      <c r="L86">
+        <v>0.00631427</v>
+      </c>
+      <c r="M86">
+        <v>0.010220101120785</v>
+      </c>
+      <c r="N86">
+        <v>0.018487102482577</v>
+      </c>
+      <c r="O86">
+        <v>0.06849482252599989</v>
+      </c>
+      <c r="P86">
+        <v>0.13888391827976</v>
+      </c>
+      <c r="Q86">
+        <v>0.19652677809815</v>
+      </c>
+      <c r="R86">
+        <v>0.24990791111325</v>
+      </c>
+      <c r="S86">
+        <v>0.29435616582149</v>
+      </c>
+      <c r="T86">
+        <v>0.33398909427959</v>
+      </c>
+    </row>
+    <row r="87" spans="1:20">
+      <c r="A87" t="s">
+        <v>20</v>
+      </c>
+      <c r="B87" t="s">
+        <v>31</v>
+      </c>
+      <c r="C87" t="s">
+        <v>53</v>
+      </c>
+      <c r="D87" t="s">
+        <v>57</v>
+      </c>
+      <c r="E87" t="s">
+        <v>59</v>
+      </c>
+      <c r="H87">
+        <v>2.30757E-05</v>
+      </c>
+      <c r="I87">
+        <v>0.000307755</v>
+      </c>
+      <c r="J87">
+        <v>0.00409259</v>
+      </c>
+      <c r="K87">
+        <v>0.00558909</v>
+      </c>
+      <c r="L87">
+        <v>0.008284348777049999</v>
+      </c>
+      <c r="M87">
+        <v>0.02979629</v>
+      </c>
+      <c r="N87">
+        <v>0.05176172891</v>
+      </c>
+      <c r="O87">
+        <v>0.097115472359</v>
+      </c>
+      <c r="P87">
+        <v>0.19642904257</v>
+      </c>
+      <c r="Q87">
+        <v>0.29049779804</v>
+      </c>
+      <c r="R87">
+        <v>0.3765447592499999</v>
+      </c>
+      <c r="S87">
+        <v>0.44770554881</v>
+      </c>
+      <c r="T87">
+        <v>0.5029339739000001</v>
+      </c>
+    </row>
+    <row r="88" spans="1:20">
+      <c r="A88" t="s">
+        <v>20</v>
+      </c>
+      <c r="B88" t="s">
+        <v>32</v>
+      </c>
+      <c r="C88" t="s">
+        <v>53</v>
+      </c>
+      <c r="D88" t="s">
+        <v>56</v>
+      </c>
+      <c r="E88" t="s">
+        <v>59</v>
+      </c>
+      <c r="F88">
+        <v>4.34442E-07</v>
+      </c>
+      <c r="G88">
+        <v>1.957485E-06</v>
+      </c>
+      <c r="H88">
+        <v>1.253057E-05</v>
+      </c>
+      <c r="I88">
+        <v>9.49463E-05</v>
+      </c>
+      <c r="J88">
+        <v>0.000618535</v>
+      </c>
+      <c r="K88">
+        <v>0.000719726113208</v>
+      </c>
+      <c r="L88">
+        <v>0.000841710232981</v>
+      </c>
+      <c r="M88">
+        <v>0.00122437682058</v>
+      </c>
+      <c r="N88">
+        <v>0.0047561749924</v>
+      </c>
+      <c r="O88">
+        <v>0.008570577896771001</v>
+      </c>
+      <c r="P88">
+        <v>0.0165685175680999</v>
+      </c>
+      <c r="Q88">
+        <v>0.024261665872572</v>
+      </c>
+      <c r="R88">
+        <v>0.034603529974589</v>
+      </c>
+      <c r="S88">
+        <v>0.041741972838302</v>
+      </c>
+      <c r="T88">
+        <v>0.0478069868787</v>
+      </c>
+    </row>
+    <row r="89" spans="1:20">
+      <c r="A89" t="s">
+        <v>20</v>
+      </c>
+      <c r="B89" t="s">
+        <v>32</v>
+      </c>
+      <c r="C89" t="s">
+        <v>53</v>
+      </c>
+      <c r="D89" t="s">
+        <v>57</v>
+      </c>
+      <c r="E89" t="s">
+        <v>59</v>
+      </c>
+      <c r="F89">
+        <v>7.46454E-09</v>
+      </c>
+      <c r="G89">
+        <v>1.03657E-07</v>
+      </c>
+      <c r="H89">
+        <v>1.77353E-06</v>
+      </c>
+      <c r="I89">
+        <v>3.33481E-05</v>
+      </c>
+      <c r="J89">
+        <v>0.00053183</v>
+      </c>
+      <c r="K89">
+        <v>0.0006633790103</v>
+      </c>
+      <c r="L89">
+        <v>0.0019187459999999</v>
+      </c>
+      <c r="M89">
+        <v>0.00314149033004</v>
+      </c>
+      <c r="N89">
+        <v>0.005343021680273</v>
+      </c>
+      <c r="O89">
+        <v>0.00991088596837</v>
+      </c>
+      <c r="P89">
+        <v>0.019623650278695</v>
+      </c>
+      <c r="Q89">
+        <v>0.028885937601483</v>
+      </c>
+      <c r="R89">
+        <v>0.0374036083255499</v>
+      </c>
+      <c r="S89">
+        <v>0.044645368688</v>
+      </c>
+      <c r="T89">
+        <v>0.05045574948</v>
+      </c>
+    </row>
+    <row r="90" spans="1:20">
+      <c r="A90" t="s">
+        <v>20</v>
+      </c>
+      <c r="B90" t="s">
+        <v>33</v>
+      </c>
+      <c r="C90" t="s">
+        <v>53</v>
+      </c>
+      <c r="D90" t="s">
+        <v>56</v>
+      </c>
+      <c r="E90" t="s">
+        <v>59</v>
+      </c>
+      <c r="F90">
+        <v>4.5649755E-08</v>
+      </c>
+      <c r="G90">
+        <v>2.0628865E-07</v>
+      </c>
+      <c r="H90">
+        <v>7.075282E-07</v>
+      </c>
+      <c r="I90">
+        <v>5.648871999999999E-06</v>
+      </c>
+      <c r="J90">
+        <v>3.79238E-05</v>
+      </c>
+      <c r="K90">
+        <v>4.824257E-05</v>
+      </c>
+      <c r="L90">
+        <v>6.40057E-05</v>
+      </c>
+      <c r="M90">
+        <v>8.62398E-05</v>
+      </c>
+      <c r="N90">
+        <v>0.0001069275</v>
+      </c>
+      <c r="O90">
+        <v>0.0001213548</v>
+      </c>
+      <c r="P90">
+        <v>0.000138328015595</v>
+      </c>
+      <c r="Q90">
+        <v>7.96091E-05</v>
+      </c>
+      <c r="R90">
+        <v>4.67847E-05</v>
+      </c>
+      <c r="S90">
+        <v>2.783683E-05</v>
+      </c>
+      <c r="T90">
+        <v>1.782634E-05</v>
+      </c>
+    </row>
+    <row r="91" spans="1:20">
+      <c r="A91" t="s">
+        <v>20</v>
+      </c>
+      <c r="B91" t="s">
+        <v>33</v>
+      </c>
+      <c r="C91" t="s">
+        <v>53</v>
+      </c>
+      <c r="D91" t="s">
+        <v>57</v>
+      </c>
+      <c r="E91" t="s">
+        <v>59</v>
+      </c>
+      <c r="F91">
+        <v>5.71478E-10</v>
+      </c>
+      <c r="G91">
+        <v>8.580470000000001E-09</v>
+      </c>
+      <c r="H91">
+        <v>9.30203E-08</v>
+      </c>
+      <c r="I91">
+        <v>1.86055E-06</v>
+      </c>
+      <c r="J91">
+        <v>3.36653E-05</v>
+      </c>
+      <c r="K91">
+        <v>4.42727E-05</v>
+      </c>
+      <c r="L91">
+        <v>6.07265E-05</v>
+      </c>
+      <c r="M91">
+        <v>8.55333E-05</v>
+      </c>
+      <c r="N91">
+        <v>0.000113461272</v>
+      </c>
+      <c r="O91">
+        <v>0.0004357169</v>
+      </c>
+      <c r="P91">
+        <v>0.0005867121</v>
+      </c>
+      <c r="Q91">
+        <v>0.0001199678442</v>
+      </c>
+      <c r="R91">
+        <v>7.756209999999999E-05</v>
+      </c>
+      <c r="S91">
+        <v>5.01301E-05</v>
+      </c>
+      <c r="T91">
+        <v>3.35481E-05</v>
+      </c>
+    </row>
+    <row r="92" spans="1:20">
+      <c r="A92" t="s">
+        <v>20</v>
+      </c>
+      <c r="B92" t="s">
+        <v>34</v>
+      </c>
+      <c r="C92" t="s">
+        <v>53</v>
+      </c>
+      <c r="D92" t="s">
+        <v>56</v>
+      </c>
+      <c r="E92" t="s">
+        <v>59</v>
+      </c>
+      <c r="F92">
+        <v>1.1792311E-07</v>
+      </c>
+      <c r="G92">
+        <v>4.32174E-07</v>
+      </c>
+      <c r="H92">
+        <v>1.619759E-06</v>
+      </c>
+      <c r="I92">
+        <v>1.431567E-05</v>
+      </c>
+      <c r="J92">
+        <v>0.0001100345</v>
+      </c>
+      <c r="K92">
+        <v>0.0001373437</v>
+      </c>
+      <c r="L92">
+        <v>0.0001729827</v>
+      </c>
+      <c r="M92">
+        <v>0.000191499</v>
+      </c>
+      <c r="N92">
+        <v>0.0001863675</v>
+      </c>
+      <c r="O92">
+        <v>0.0001969497</v>
+      </c>
+      <c r="P92">
+        <v>0.000216762</v>
+      </c>
+      <c r="Q92">
+        <v>0.0001151612</v>
+      </c>
+      <c r="R92">
+        <v>6.34419E-05</v>
+      </c>
+      <c r="S92">
+        <v>3.69998E-05</v>
+      </c>
+      <c r="T92">
+        <v>2.33574E-05</v>
+      </c>
+    </row>
+    <row r="93" spans="1:20">
+      <c r="A93" t="s">
+        <v>20</v>
+      </c>
+      <c r="B93" t="s">
+        <v>34</v>
+      </c>
+      <c r="C93" t="s">
+        <v>53</v>
+      </c>
+      <c r="D93" t="s">
+        <v>57</v>
+      </c>
+      <c r="E93" t="s">
+        <v>59</v>
+      </c>
+      <c r="F93">
+        <v>2.07457E-09</v>
+      </c>
+      <c r="G93">
+        <v>2.90154E-08</v>
+      </c>
+      <c r="H93">
+        <v>3.27722E-07</v>
+      </c>
+      <c r="I93">
+        <v>7.01475E-06</v>
+      </c>
+      <c r="J93">
+        <v>0.000134121</v>
+      </c>
+      <c r="K93">
+        <v>0.000170547</v>
+      </c>
+      <c r="L93">
+        <v>0.000219865</v>
+      </c>
+      <c r="M93">
+        <v>0.000257355</v>
+      </c>
+      <c r="N93">
+        <v>0.000269023232064</v>
+      </c>
+      <c r="O93">
+        <v>0.00030522854045</v>
+      </c>
+      <c r="P93">
+        <v>0.00036437408621</v>
+      </c>
+      <c r="Q93">
+        <v>0.000209943</v>
+      </c>
+      <c r="R93">
+        <v>0.000124309</v>
+      </c>
+      <c r="S93">
+        <v>7.565130000000001E-05</v>
+      </c>
+      <c r="T93">
+        <v>4.84768E-05</v>
+      </c>
+    </row>
+    <row r="94" spans="1:20">
+      <c r="A94" t="s">
+        <v>20</v>
+      </c>
+      <c r="B94" t="s">
+        <v>35</v>
+      </c>
+      <c r="C94" t="s">
+        <v>53</v>
+      </c>
+      <c r="D94" t="s">
+        <v>56</v>
+      </c>
+      <c r="E94" t="s">
+        <v>59</v>
+      </c>
+      <c r="H94">
+        <v>1.1112593E-06</v>
+      </c>
+      <c r="I94">
+        <v>6.342823E-06</v>
+      </c>
+      <c r="J94">
+        <v>4.119778E-05</v>
+      </c>
+      <c r="K94">
+        <v>4.976658E-05</v>
+      </c>
+      <c r="L94">
+        <v>6.058184E-05</v>
+      </c>
+      <c r="M94">
+        <v>6.495660000000001E-05</v>
+      </c>
+      <c r="N94">
+        <v>5.76946E-05</v>
+      </c>
+      <c r="O94">
+        <v>5.47918E-05</v>
+      </c>
+      <c r="P94">
+        <v>5.27197E-05</v>
+      </c>
+      <c r="Q94">
+        <v>2.649625E-05</v>
+      </c>
+      <c r="R94">
+        <v>1.402328E-05</v>
+      </c>
+      <c r="S94">
+        <v>7.80991E-06</v>
+      </c>
+      <c r="T94">
+        <v>4.87287E-06</v>
+      </c>
+    </row>
+    <row r="95" spans="1:20">
+      <c r="A95" t="s">
+        <v>20</v>
+      </c>
+      <c r="B95" t="s">
+        <v>35</v>
+      </c>
+      <c r="C95" t="s">
+        <v>53</v>
+      </c>
+      <c r="D95" t="s">
+        <v>57</v>
+      </c>
+      <c r="E95" t="s">
+        <v>59</v>
+      </c>
+      <c r="H95">
+        <v>1.47805E-07</v>
+      </c>
+      <c r="I95">
+        <v>2.159E-06</v>
+      </c>
+      <c r="J95">
+        <v>3.50159E-05</v>
+      </c>
+      <c r="K95">
+        <v>4.29476E-05</v>
+      </c>
+      <c r="L95">
+        <v>5.42134E-05</v>
+      </c>
+      <c r="M95">
+        <v>6.28625E-05</v>
+      </c>
+      <c r="N95">
+        <v>6.30802E-05</v>
+      </c>
+      <c r="O95">
+        <v>6.857160000000001E-05</v>
+      </c>
+      <c r="P95">
+        <v>7.70959E-05</v>
+      </c>
+      <c r="Q95">
+        <v>4.46803E-05</v>
+      </c>
+      <c r="R95">
+        <v>2.69854E-05</v>
+      </c>
+      <c r="S95">
+        <v>1.68037E-05</v>
+      </c>
+      <c r="T95">
+        <v>1.12578E-05</v>
+      </c>
+    </row>
+    <row r="96" spans="1:20">
+      <c r="A96" t="s">
+        <v>20</v>
+      </c>
+      <c r="B96" t="s">
+        <v>36</v>
+      </c>
+      <c r="C96" t="s">
+        <v>53</v>
+      </c>
+      <c r="D96" t="s">
+        <v>56</v>
+      </c>
+      <c r="E96" t="s">
+        <v>59</v>
+      </c>
+      <c r="F96">
+        <v>1.7158697E-08</v>
+      </c>
+      <c r="G96">
+        <v>6.62908E-08</v>
+      </c>
+      <c r="H96">
+        <v>2.523171E-07</v>
+      </c>
+      <c r="I96">
+        <v>1.71296E-06</v>
+      </c>
+      <c r="J96">
+        <v>1.346397E-05</v>
+      </c>
+      <c r="K96">
+        <v>1.909386E-05</v>
+      </c>
+      <c r="L96">
+        <v>2.72523E-05</v>
+      </c>
+      <c r="M96">
+        <v>3.99925E-05</v>
+      </c>
+      <c r="N96">
+        <v>6.2035639368E-05</v>
+      </c>
+      <c r="O96">
+        <v>0.0001426196</v>
+      </c>
+      <c r="P96">
+        <v>0.00023259327025</v>
+      </c>
+      <c r="Q96">
+        <v>6.3250255549E-05</v>
+      </c>
+      <c r="R96">
+        <v>3.56322E-05</v>
+      </c>
+      <c r="S96">
+        <v>2.052973E-05</v>
+      </c>
+      <c r="T96">
+        <v>1.218989E-05</v>
+      </c>
+    </row>
+    <row r="97" spans="1:20">
+      <c r="A97" t="s">
+        <v>20</v>
+      </c>
+      <c r="B97" t="s">
+        <v>36</v>
+      </c>
+      <c r="C97" t="s">
+        <v>53</v>
+      </c>
+      <c r="D97" t="s">
+        <v>57</v>
+      </c>
+      <c r="E97" t="s">
+        <v>59</v>
+      </c>
+      <c r="F97">
+        <v>4.73628E-10</v>
+      </c>
+      <c r="G97">
+        <v>7.0512E-09</v>
+      </c>
+      <c r="H97">
+        <v>7.012439999999999E-08</v>
+      </c>
+      <c r="I97">
+        <v>1.04503E-06</v>
+      </c>
+      <c r="J97">
+        <v>1.84099E-05</v>
+      </c>
+      <c r="K97">
+        <v>2.71397E-05</v>
+      </c>
+      <c r="L97">
+        <v>8.214439999999999E-05</v>
+      </c>
+      <c r="M97">
+        <v>0.000136297046712</v>
+      </c>
+      <c r="N97">
+        <v>0.000219663986</v>
+      </c>
+      <c r="O97">
+        <v>0.0003380461567</v>
+      </c>
+      <c r="P97">
+        <v>0.0004800576427</v>
+      </c>
+      <c r="Q97">
+        <v>0.000544214271</v>
+      </c>
+      <c r="R97">
+        <v>0.0005550220885</v>
+      </c>
+      <c r="S97">
+        <v>3.421631891E-05</v>
+      </c>
+      <c r="T97">
+        <v>2.00523E-05</v>
+      </c>
+    </row>
+    <row r="98" spans="1:20">
+      <c r="A98" t="s">
+        <v>20</v>
+      </c>
+      <c r="B98" t="s">
+        <v>37</v>
+      </c>
+      <c r="C98" t="s">
+        <v>53</v>
+      </c>
+      <c r="D98" t="s">
+        <v>56</v>
+      </c>
+      <c r="E98" t="s">
+        <v>59</v>
+      </c>
+      <c r="F98">
+        <v>5.242717999999999E-08</v>
+      </c>
+      <c r="G98">
+        <v>1.9192604E-07</v>
+      </c>
+      <c r="H98">
+        <v>1.5532309E-06</v>
+      </c>
+      <c r="I98">
+        <v>9.944658E-06</v>
+      </c>
+      <c r="J98">
+        <v>5.777333E-05</v>
+      </c>
+      <c r="K98">
+        <v>6.249672E-05</v>
+      </c>
+      <c r="L98">
+        <v>4.790184000000001E-05</v>
+      </c>
+      <c r="M98">
+        <v>3.711694E-05</v>
+      </c>
+      <c r="N98">
+        <v>2.997544E-05</v>
+      </c>
+      <c r="O98">
+        <v>2.711607E-05</v>
+      </c>
+      <c r="P98">
+        <v>2.743675E-05</v>
+      </c>
+      <c r="Q98">
+        <v>1.513087E-05</v>
+      </c>
+      <c r="R98">
+        <v>9.182459999999999E-06</v>
+      </c>
+      <c r="S98">
+        <v>5.955400000000001E-06</v>
+      </c>
+      <c r="T98">
+        <v>4.29831E-06</v>
+      </c>
+    </row>
+    <row r="99" spans="1:20">
+      <c r="A99" t="s">
+        <v>20</v>
+      </c>
+      <c r="B99" t="s">
+        <v>37</v>
+      </c>
+      <c r="C99" t="s">
+        <v>53</v>
+      </c>
+      <c r="D99" t="s">
+        <v>57</v>
+      </c>
+      <c r="E99" t="s">
+        <v>59</v>
+      </c>
+      <c r="F99">
+        <v>8.70256E-10</v>
+      </c>
+      <c r="G99">
+        <v>1.06552E-08</v>
+      </c>
+      <c r="H99">
+        <v>2.10243E-07</v>
+      </c>
+      <c r="I99">
+        <v>3.63288E-06</v>
+      </c>
+      <c r="J99">
+        <v>5.92676E-05</v>
+      </c>
+      <c r="K99">
+        <v>6.600950000000001E-05</v>
+      </c>
+      <c r="L99">
+        <v>5.66134E-05</v>
+      </c>
+      <c r="M99">
+        <v>4.9382E-05</v>
+      </c>
+      <c r="N99">
+        <v>4.75565E-05</v>
+      </c>
+      <c r="O99">
+        <v>5.18353E-05</v>
+      </c>
+      <c r="P99">
+        <v>6.01037E-05</v>
+      </c>
+      <c r="Q99">
+        <v>3.73036E-05</v>
+      </c>
+      <c r="R99">
+        <v>2.48021E-05</v>
+      </c>
+      <c r="S99">
+        <v>1.69609E-05</v>
+      </c>
+      <c r="T99">
+        <v>1.24427E-05</v>
+      </c>
+    </row>
+    <row r="100" spans="1:20">
+      <c r="A100" t="s">
+        <v>20</v>
+      </c>
+      <c r="B100" t="s">
+        <v>38</v>
+      </c>
+      <c r="C100" t="s">
+        <v>53</v>
+      </c>
+      <c r="D100" t="s">
+        <v>56</v>
+      </c>
+      <c r="E100" t="s">
+        <v>59</v>
+      </c>
+      <c r="F100">
+        <v>2.4434681E-08</v>
+      </c>
+      <c r="G100">
+        <v>8.064521E-08</v>
+      </c>
+      <c r="H100">
+        <v>4.618762E-07</v>
+      </c>
+      <c r="I100">
+        <v>2.622583E-06</v>
+      </c>
+      <c r="J100">
+        <v>1.515964E-05</v>
+      </c>
+      <c r="K100">
+        <v>1.516137E-05</v>
+      </c>
+      <c r="L100">
+        <v>9.296639999999999E-06</v>
+      </c>
+      <c r="M100">
+        <v>5.482684E-06</v>
+      </c>
+      <c r="N100">
+        <v>3.513546E-06</v>
+      </c>
+      <c r="O100">
+        <v>2.844306E-06</v>
+      </c>
+      <c r="P100">
+        <v>2.611071E-06</v>
+      </c>
+      <c r="Q100">
+        <v>1.334914E-06</v>
+      </c>
+      <c r="R100">
+        <v>7.42511E-07</v>
+      </c>
+      <c r="S100">
+        <v>4.45502E-07</v>
+      </c>
+      <c r="T100">
+        <v>2.92829E-07</v>
+      </c>
+    </row>
+    <row r="101" spans="1:20">
+      <c r="A101" t="s">
+        <v>20</v>
+      </c>
+      <c r="B101" t="s">
+        <v>38</v>
+      </c>
+      <c r="C101" t="s">
+        <v>53</v>
+      </c>
+      <c r="D101" t="s">
+        <v>57</v>
+      </c>
+      <c r="E101" t="s">
+        <v>59</v>
+      </c>
+      <c r="F101">
+        <v>2.44473E-10</v>
+      </c>
+      <c r="G101">
+        <v>2.97996E-09</v>
+      </c>
+      <c r="H101">
+        <v>4.78101E-08</v>
+      </c>
+      <c r="I101">
+        <v>8.18225E-07</v>
+      </c>
+      <c r="J101">
+        <v>1.32846E-05</v>
+      </c>
+      <c r="K101">
+        <v>1.46006E-05</v>
+      </c>
+      <c r="L101">
+        <v>1.11002E-05</v>
+      </c>
+      <c r="M101">
+        <v>8.54768E-06</v>
+      </c>
+      <c r="N101">
+        <v>7.10191E-06</v>
+      </c>
+      <c r="O101">
+        <v>6.74595E-06</v>
+      </c>
+      <c r="P101">
+        <v>6.77962E-06</v>
+      </c>
+      <c r="Q101">
+        <v>3.71569E-06</v>
+      </c>
+      <c r="R101">
+        <v>2.20199E-06</v>
+      </c>
+      <c r="S101">
+        <v>1.38561E-06</v>
+      </c>
+      <c r="T101">
+        <v>9.36071E-07</v>
+      </c>
+    </row>
+    <row r="102" spans="1:20">
+      <c r="A102" t="s">
+        <v>20</v>
+      </c>
+      <c r="B102" t="s">
+        <v>39</v>
+      </c>
+      <c r="C102" t="s">
+        <v>53</v>
+      </c>
+      <c r="D102" t="s">
+        <v>56</v>
+      </c>
+      <c r="E102" t="s">
+        <v>59</v>
+      </c>
+      <c r="F102">
+        <v>8.130935E-08</v>
+      </c>
+      <c r="G102">
+        <v>4.421999E-07</v>
+      </c>
+      <c r="H102">
+        <v>2.483883E-06</v>
+      </c>
+      <c r="I102">
+        <v>1.844228E-05</v>
+      </c>
+      <c r="J102">
+        <v>0.0001366191</v>
+      </c>
+      <c r="K102">
+        <v>0.0001766959</v>
+      </c>
+      <c r="L102">
+        <v>0.0002420966</v>
+      </c>
+      <c r="M102">
+        <v>0.0003514442</v>
+      </c>
+      <c r="N102">
+        <v>0.000560878962</v>
+      </c>
+      <c r="O102">
+        <v>0.002078755199916</v>
+      </c>
+      <c r="P102">
+        <v>0.003282855090875</v>
+      </c>
+      <c r="Q102">
+        <v>0.00382039657</v>
+      </c>
+      <c r="R102">
+        <v>0.0030539560999999</v>
+      </c>
+      <c r="S102">
+        <v>0.0004977569641940001</v>
+      </c>
+      <c r="T102">
+        <v>0.000352422</v>
+      </c>
+    </row>
+    <row r="103" spans="1:20">
+      <c r="A103" t="s">
+        <v>20</v>
+      </c>
+      <c r="B103" t="s">
+        <v>39</v>
+      </c>
+      <c r="C103" t="s">
+        <v>53</v>
+      </c>
+      <c r="D103" t="s">
+        <v>57</v>
+      </c>
+      <c r="E103" t="s">
+        <v>59</v>
+      </c>
+      <c r="F103">
+        <v>1.75322E-09</v>
+      </c>
+      <c r="G103">
+        <v>2.75669E-08</v>
+      </c>
+      <c r="H103">
+        <v>4.16726E-07</v>
+      </c>
+      <c r="I103">
+        <v>7.52554E-06</v>
+      </c>
+      <c r="J103">
+        <v>0.00013441</v>
+      </c>
+      <c r="K103">
+        <v>0.000177603</v>
+      </c>
+      <c r="L103">
+        <v>0.000249101112154</v>
+      </c>
+      <c r="M103">
+        <v>0.00037422046</v>
+      </c>
+      <c r="N103">
+        <v>0.001446069813974</v>
+      </c>
+      <c r="O103">
+        <v>0.00248157181</v>
+      </c>
+      <c r="P103">
+        <v>0.004195336568</v>
+      </c>
+      <c r="Q103">
+        <v>0.00531561433106</v>
+      </c>
+      <c r="R103">
+        <v>0.00595145137</v>
+      </c>
+      <c r="S103">
+        <v>0.006180382663</v>
+      </c>
+      <c r="T103">
+        <v>0.0060816538</v>
+      </c>
+    </row>
+    <row r="104" spans="1:20">
+      <c r="A104" t="s">
+        <v>20</v>
+      </c>
+      <c r="B104" t="s">
+        <v>40</v>
+      </c>
+      <c r="C104" t="s">
+        <v>53</v>
+      </c>
+      <c r="D104" t="s">
+        <v>56</v>
+      </c>
+      <c r="E104" t="s">
+        <v>59</v>
+      </c>
+      <c r="F104">
+        <v>8.131649000000001E-07</v>
+      </c>
+      <c r="G104">
+        <v>3.573748E-06</v>
+      </c>
+      <c r="H104">
+        <v>2.390692E-05</v>
+      </c>
+      <c r="I104">
+        <v>0.0001675661</v>
+      </c>
+      <c r="J104">
+        <v>0.001007323</v>
+      </c>
+      <c r="K104">
+        <v>0.0011183311207979</v>
+      </c>
+      <c r="L104">
+        <v>0.00146728984135</v>
+      </c>
+      <c r="M104">
+        <v>0.005244277085699999</v>
+      </c>
+      <c r="N104">
+        <v>0.00906202117158</v>
+      </c>
+      <c r="O104">
+        <v>0.016358246485411</v>
+      </c>
+      <c r="P104">
+        <v>0.03081556030145</v>
+      </c>
+      <c r="Q104">
+        <v>0.04232982552719</v>
+      </c>
+      <c r="R104">
+        <v>0.0525532537267799</v>
+      </c>
+      <c r="S104">
+        <v>0.0608576464721339</v>
+      </c>
+      <c r="T104">
+        <v>0.06751777048663191</v>
+      </c>
+    </row>
+    <row r="105" spans="1:20">
+      <c r="A105" t="s">
+        <v>20</v>
+      </c>
+      <c r="B105" t="s">
+        <v>40</v>
+      </c>
+      <c r="C105" t="s">
+        <v>53</v>
+      </c>
+      <c r="D105" t="s">
+        <v>57</v>
+      </c>
+      <c r="E105" t="s">
+        <v>59</v>
+      </c>
+      <c r="F105">
+        <v>1.37047E-08</v>
+      </c>
+      <c r="G105">
+        <v>1.7272E-07</v>
+      </c>
+      <c r="H105">
+        <v>2.86239E-06</v>
+      </c>
+      <c r="I105">
+        <v>4.96605E-05</v>
+      </c>
+      <c r="J105">
+        <v>0.000763371</v>
+      </c>
+      <c r="K105">
+        <v>0.000905120891955</v>
+      </c>
+      <c r="L105">
+        <v>0.001242822564</v>
+      </c>
+      <c r="M105">
+        <v>0.00469414931444</v>
+      </c>
+      <c r="N105">
+        <v>0.0081627241999999</v>
+      </c>
+      <c r="O105">
+        <v>0.01521058115</v>
+      </c>
+      <c r="P105">
+        <v>0.029937410663291</v>
+      </c>
+      <c r="Q105">
+        <v>0.043691780072433</v>
+      </c>
+      <c r="R105">
+        <v>0.0560069421194</v>
+      </c>
+      <c r="S105">
+        <v>0.066027849931</v>
+      </c>
+      <c r="T105">
+        <v>0.07362466301999999</v>
+      </c>
+    </row>
+    <row r="106" spans="1:20">
+      <c r="A106" t="s">
+        <v>20</v>
+      </c>
+      <c r="B106" t="s">
+        <v>41</v>
+      </c>
+      <c r="C106" t="s">
+        <v>53</v>
+      </c>
+      <c r="D106" t="s">
+        <v>56</v>
+      </c>
+      <c r="E106" t="s">
+        <v>59</v>
+      </c>
+      <c r="F106">
+        <v>8.020182E-07</v>
+      </c>
+      <c r="G106">
+        <v>3.102619E-06</v>
+      </c>
+      <c r="H106">
+        <v>1.7828446E-05</v>
+      </c>
+      <c r="I106">
+        <v>0.00010047188</v>
+      </c>
+      <c r="J106">
+        <v>0.0006920168</v>
+      </c>
+      <c r="K106">
+        <v>0.0009811749999999999</v>
+      </c>
+      <c r="L106">
+        <v>0.001472169</v>
+      </c>
+      <c r="M106">
+        <v>0.0022572472401</v>
+      </c>
+      <c r="N106">
+        <v>0.008262220745742</v>
+      </c>
+      <c r="O106">
+        <v>0.014363555076</v>
+      </c>
+      <c r="P106">
+        <v>0.025200435115</v>
+      </c>
+      <c r="Q106">
+        <v>0.033523885568724</v>
+      </c>
+      <c r="R106">
+        <v>0.038458921771</v>
+      </c>
+      <c r="S106">
+        <v>0.040726315622</v>
+      </c>
+      <c r="T106">
+        <v>0.04118473347721999</v>
+      </c>
+    </row>
+    <row r="107" spans="1:20">
+      <c r="A107" t="s">
+        <v>20</v>
+      </c>
+      <c r="B107" t="s">
+        <v>41</v>
+      </c>
+      <c r="C107" t="s">
+        <v>53</v>
+      </c>
+      <c r="D107" t="s">
+        <v>57</v>
+      </c>
+      <c r="E107" t="s">
+        <v>59</v>
+      </c>
+      <c r="F107">
+        <v>9.58765E-09</v>
+      </c>
+      <c r="G107">
+        <v>1.19914E-07</v>
+      </c>
+      <c r="H107">
+        <v>1.90688E-06</v>
+      </c>
+      <c r="I107">
+        <v>2.97422E-05</v>
+      </c>
+      <c r="J107">
+        <v>0.000543824</v>
+      </c>
+      <c r="K107">
+        <v>0.000789758</v>
+      </c>
+      <c r="L107">
+        <v>0.001221940695806</v>
+      </c>
+      <c r="M107">
+        <v>0.0020068012</v>
+      </c>
+      <c r="N107">
+        <v>0.00734573733679</v>
+      </c>
+      <c r="O107">
+        <v>0.013214892149344</v>
+      </c>
+      <c r="P107">
+        <v>0.024352621511</v>
+      </c>
+      <c r="Q107">
+        <v>0.033974198891</v>
+      </c>
+      <c r="R107">
+        <v>0.040240313023</v>
+      </c>
+      <c r="S107">
+        <v>0.04321608069</v>
+      </c>
+      <c r="T107">
+        <v>0.04347077389</v>
+      </c>
+    </row>
+    <row r="108" spans="1:20">
+      <c r="A108" t="s">
+        <v>20</v>
+      </c>
+      <c r="B108" t="s">
+        <v>42</v>
+      </c>
+      <c r="C108" t="s">
+        <v>53</v>
+      </c>
+      <c r="D108" t="s">
+        <v>56</v>
+      </c>
+      <c r="E108" t="s">
+        <v>59</v>
+      </c>
+      <c r="H108">
+        <v>1.667413E-07</v>
+      </c>
+      <c r="I108">
+        <v>1.097921E-06</v>
+      </c>
+      <c r="J108">
+        <v>5.495777E-06</v>
+      </c>
+      <c r="K108">
+        <v>4.020124000000001E-06</v>
+      </c>
+      <c r="L108">
+        <v>1.868128E-06</v>
+      </c>
+      <c r="M108">
+        <v>8.50225E-07</v>
+      </c>
+      <c r="N108">
+        <v>4.169657E-07</v>
+      </c>
+      <c r="O108">
+        <v>2.353403E-07</v>
+      </c>
+      <c r="P108">
+        <v>1.378918E-07</v>
+      </c>
+      <c r="Q108">
+        <v>4.91201E-08</v>
+      </c>
+      <c r="R108">
+        <v>2.053137E-08</v>
+      </c>
+      <c r="S108">
+        <v>9.9158E-09</v>
+      </c>
+      <c r="T108">
+        <v>5.256440000000001E-09</v>
+      </c>
+    </row>
+    <row r="109" spans="1:20">
+      <c r="A109" t="s">
+        <v>20</v>
+      </c>
+      <c r="B109" t="s">
+        <v>42</v>
+      </c>
+      <c r="C109" t="s">
+        <v>53</v>
+      </c>
+      <c r="D109" t="s">
+        <v>57</v>
+      </c>
+      <c r="E109" t="s">
+        <v>59</v>
+      </c>
+      <c r="H109">
+        <v>2.77371E-08</v>
+      </c>
+      <c r="I109">
+        <v>4.7448E-07</v>
+      </c>
+      <c r="J109">
+        <v>6.682E-06</v>
+      </c>
+      <c r="K109">
+        <v>5.6087E-06</v>
+      </c>
+      <c r="L109">
+        <v>3.28919E-06</v>
+      </c>
+      <c r="M109">
+        <v>1.90896E-06</v>
+      </c>
+      <c r="N109">
+        <v>1.20314E-06</v>
+      </c>
+      <c r="O109">
+        <v>8.63253E-07</v>
+      </c>
+      <c r="P109">
+        <v>6.43401E-07</v>
+      </c>
+      <c r="Q109">
+        <v>2.7896E-07</v>
+      </c>
+      <c r="R109">
+        <v>1.34571E-07</v>
+      </c>
+      <c r="S109">
+        <v>7.164969999999999E-08</v>
+      </c>
+      <c r="T109">
+        <v>4.07422E-08</v>
+      </c>
+    </row>
+    <row r="110" spans="1:20">
+      <c r="A110" t="s">
+        <v>20</v>
+      </c>
+      <c r="B110" t="s">
+        <v>43</v>
+      </c>
+      <c r="C110" t="s">
+        <v>53</v>
+      </c>
+      <c r="D110" t="s">
+        <v>56</v>
+      </c>
+      <c r="E110" t="s">
+        <v>59</v>
+      </c>
+      <c r="H110">
+        <v>2.696932E-05</v>
+      </c>
+      <c r="I110">
+        <v>0.0001595193</v>
+      </c>
+      <c r="J110">
+        <v>0.000856312</v>
+      </c>
+      <c r="K110">
+        <v>0.001267533</v>
+      </c>
+      <c r="L110">
+        <v>0.0019115824909999</v>
+      </c>
+      <c r="M110">
+        <v>0.0063042150738</v>
+      </c>
+      <c r="N110">
+        <v>0.010883929</v>
+      </c>
+      <c r="O110">
+        <v>0.0192162472</v>
+      </c>
+      <c r="P110">
+        <v>0.0343259957211199</v>
+      </c>
+      <c r="Q110">
+        <v>0.045255410314224</v>
+      </c>
+      <c r="R110">
+        <v>0.053629381149933</v>
+      </c>
+      <c r="S110">
+        <v>0.058988500938157</v>
+      </c>
+      <c r="T110">
+        <v>0.0610916540666589</v>
+      </c>
+    </row>
+    <row r="111" spans="1:20">
+      <c r="A111" t="s">
+        <v>20</v>
+      </c>
+      <c r="B111" t="s">
+        <v>43</v>
+      </c>
+      <c r="C111" t="s">
+        <v>53</v>
+      </c>
+      <c r="D111" t="s">
+        <v>57</v>
+      </c>
+      <c r="E111" t="s">
+        <v>59</v>
+      </c>
+      <c r="H111">
+        <v>2.55507E-06</v>
+      </c>
+      <c r="I111">
+        <v>4.2474E-05</v>
+      </c>
+      <c r="J111">
+        <v>0.000626813</v>
+      </c>
+      <c r="K111">
+        <v>0.000948277</v>
+      </c>
+      <c r="L111">
+        <v>0.0014563967468</v>
+      </c>
+      <c r="M111">
+        <v>0.005153151</v>
+      </c>
+      <c r="N111">
+        <v>0.009055908</v>
+      </c>
+      <c r="O111">
+        <v>0.016696744328</v>
+      </c>
+      <c r="P111">
+        <v>0.031772514795</v>
+      </c>
+      <c r="Q111">
+        <v>0.044904280366</v>
+      </c>
+      <c r="R111">
+        <v>0.055531757238</v>
+      </c>
+      <c r="S111">
+        <v>0.062804433703</v>
+      </c>
+      <c r="T111">
+        <v>0.06593970011</v>
+      </c>
+    </row>
+    <row r="112" spans="1:20">
+      <c r="A112" t="s">
+        <v>20</v>
+      </c>
+      <c r="B112" t="s">
+        <v>44</v>
+      </c>
+      <c r="C112" t="s">
+        <v>53</v>
+      </c>
+      <c r="D112" t="s">
+        <v>56</v>
+      </c>
+      <c r="E112" t="s">
+        <v>59</v>
+      </c>
+      <c r="F112">
+        <v>8.650723E-09</v>
+      </c>
+      <c r="G112">
+        <v>2.78489E-08</v>
+      </c>
+      <c r="H112">
+        <v>1.205417E-07</v>
+      </c>
+      <c r="I112">
+        <v>8.33983E-07</v>
+      </c>
+      <c r="J112">
+        <v>4.754323E-06</v>
+      </c>
+      <c r="K112">
+        <v>4.695073E-06</v>
+      </c>
+      <c r="L112">
+        <v>3.073728E-06</v>
+      </c>
+      <c r="M112">
+        <v>2.111346E-06</v>
+      </c>
+      <c r="N112">
+        <v>1.63266E-06</v>
+      </c>
+      <c r="O112">
+        <v>1.475784E-06</v>
+      </c>
+      <c r="P112">
+        <v>1.428401E-06</v>
+      </c>
+      <c r="Q112">
+        <v>7.502700000000001E-07</v>
+      </c>
+      <c r="R112">
+        <v>4.32318E-07</v>
+      </c>
+      <c r="S112">
+        <v>2.63227E-07</v>
+      </c>
+      <c r="T112">
+        <v>1.721878E-07</v>
+      </c>
+    </row>
+    <row r="113" spans="1:20">
+      <c r="A113" t="s">
+        <v>20</v>
+      </c>
+      <c r="B113" t="s">
+        <v>44</v>
+      </c>
+      <c r="C113" t="s">
+        <v>53</v>
+      </c>
+      <c r="D113" t="s">
+        <v>57</v>
+      </c>
+      <c r="E113" t="s">
+        <v>59</v>
+      </c>
+      <c r="F113">
+        <v>3.29988E-10</v>
+      </c>
+      <c r="G113">
+        <v>3.0603E-09</v>
+      </c>
+      <c r="H113">
+        <v>2.98839E-08</v>
+      </c>
+      <c r="I113">
+        <v>4.06623E-07</v>
+      </c>
+      <c r="J113">
+        <v>5.44308E-06</v>
+      </c>
+      <c r="K113">
+        <v>5.56273E-06</v>
+      </c>
+      <c r="L113">
+        <v>4.1707E-06</v>
+      </c>
+      <c r="M113">
+        <v>3.30833E-06</v>
+      </c>
+      <c r="N113">
+        <v>2.96101E-06</v>
+      </c>
+      <c r="O113">
+        <v>3.11359E-06</v>
+      </c>
+      <c r="P113">
+        <v>3.46714E-06</v>
+      </c>
+      <c r="Q113">
+        <v>2.05319E-06</v>
+      </c>
+      <c r="R113">
+        <v>1.30095E-06</v>
+      </c>
+      <c r="S113">
+        <v>8.50915E-07</v>
+      </c>
+      <c r="T113">
+        <v>5.87105E-07</v>
+      </c>
+    </row>
+    <row r="114" spans="1:20">
+      <c r="A114" t="s">
+        <v>20</v>
+      </c>
+      <c r="B114" t="s">
+        <v>45</v>
+      </c>
+      <c r="C114" t="s">
+        <v>53</v>
+      </c>
+      <c r="D114" t="s">
+        <v>56</v>
+      </c>
+      <c r="E114" t="s">
+        <v>59</v>
+      </c>
+      <c r="F114">
+        <v>2.3696618E-07</v>
+      </c>
+      <c r="G114">
+        <v>9.538357E-07</v>
+      </c>
+      <c r="H114">
+        <v>6.384334000000001E-06</v>
+      </c>
+      <c r="I114">
+        <v>4.753735E-05</v>
+      </c>
+      <c r="J114">
+        <v>0.0003114457</v>
+      </c>
+      <c r="K114">
+        <v>0.0003929038</v>
+      </c>
+      <c r="L114">
+        <v>0.0005340496</v>
+      </c>
+      <c r="M114">
+        <v>0.00087912969931</v>
+      </c>
+      <c r="N114">
+        <v>0.00341944191216</v>
+      </c>
+      <c r="O114">
+        <v>0.006291242468582</v>
+      </c>
+      <c r="P114">
+        <v>0.0118645275971999</v>
+      </c>
+      <c r="Q114">
+        <v>0.0167350478747</v>
+      </c>
+      <c r="R114">
+        <v>0.02145815428889</v>
+      </c>
+      <c r="S114">
+        <v>0.025836272428587</v>
+      </c>
+      <c r="T114">
+        <v>0.029805726668793</v>
+      </c>
+    </row>
+    <row r="115" spans="1:20">
+      <c r="A115" t="s">
+        <v>20</v>
+      </c>
+      <c r="B115" t="s">
+        <v>45</v>
+      </c>
+      <c r="C115" t="s">
+        <v>53</v>
+      </c>
+      <c r="D115" t="s">
+        <v>57</v>
+      </c>
+      <c r="E115" t="s">
+        <v>59</v>
+      </c>
+      <c r="F115">
+        <v>1.06606E-09</v>
+      </c>
+      <c r="G115">
+        <v>1.76018E-08</v>
+      </c>
+      <c r="H115">
+        <v>4.15273E-07</v>
+      </c>
+      <c r="I115">
+        <v>1.02035E-05</v>
+      </c>
+      <c r="J115">
+        <v>0.000210574</v>
+      </c>
+      <c r="K115">
+        <v>0.000291307</v>
+      </c>
+      <c r="L115">
+        <v>0.000450631</v>
+      </c>
+      <c r="M115">
+        <v>0.0008031579888</v>
+      </c>
+      <c r="N115">
+        <v>0.003110083</v>
+      </c>
+      <c r="O115">
+        <v>0.00606730832</v>
+      </c>
+      <c r="P115">
+        <v>0.0121744831469999</v>
+      </c>
+      <c r="Q115">
+        <v>0.018080487896</v>
+      </c>
+      <c r="R115">
+        <v>0.0240292588756</v>
+      </c>
+      <c r="S115">
+        <v>0.0297485518492</v>
+      </c>
+      <c r="T115">
+        <v>0.034911641609</v>
+      </c>
+    </row>
+    <row r="116" spans="1:20">
+      <c r="A116" t="s">
+        <v>20</v>
+      </c>
+      <c r="B116" t="s">
+        <v>46</v>
+      </c>
+      <c r="C116" t="s">
+        <v>53</v>
+      </c>
+      <c r="D116" t="s">
+        <v>56</v>
+      </c>
+      <c r="E116" t="s">
+        <v>59</v>
+      </c>
+      <c r="F116">
+        <v>1.2183355E-06</v>
+      </c>
+      <c r="G116">
+        <v>5.971624E-06</v>
+      </c>
+      <c r="H116">
+        <v>4.417762E-05</v>
+      </c>
+      <c r="I116">
+        <v>0.000346727</v>
+      </c>
+      <c r="J116">
+        <v>0.002485752</v>
+      </c>
+      <c r="K116">
+        <v>0.00309180847643</v>
+      </c>
+      <c r="L116">
+        <v>0.003924358860911</v>
+      </c>
+      <c r="M116">
+        <v>0.0058808521347</v>
+      </c>
+      <c r="N116">
+        <v>0.018398441025</v>
+      </c>
+      <c r="O116">
+        <v>0.0323627727423499</v>
+      </c>
+      <c r="P116">
+        <v>0.074063287363365</v>
+      </c>
+      <c r="Q116">
+        <v>0.10881334510251</v>
+      </c>
+      <c r="R116">
+        <v>0.142026936472074</v>
+      </c>
+      <c r="S116">
+        <v>0.172224659078981</v>
+      </c>
+      <c r="T116">
+        <v>0.198390363756303</v>
+      </c>
+    </row>
+    <row r="117" spans="1:20">
+      <c r="A117" t="s">
+        <v>20</v>
+      </c>
+      <c r="B117" t="s">
+        <v>46</v>
+      </c>
+      <c r="C117" t="s">
+        <v>53</v>
+      </c>
+      <c r="D117" t="s">
+        <v>57</v>
+      </c>
+      <c r="E117" t="s">
+        <v>59</v>
+      </c>
+      <c r="F117">
+        <v>2.179E-08</v>
+      </c>
+      <c r="G117">
+        <v>3.42594E-07</v>
+      </c>
+      <c r="H117">
+        <v>6.97307E-06</v>
+      </c>
+      <c r="I117">
+        <v>0.00013761</v>
+      </c>
+      <c r="J117">
+        <v>0.00231392</v>
+      </c>
+      <c r="K117">
+        <v>0.00526966</v>
+      </c>
+      <c r="L117">
+        <v>0.009099856897369999</v>
+      </c>
+      <c r="M117">
+        <v>0.014260235</v>
+      </c>
+      <c r="N117">
+        <v>0.02319969685</v>
+      </c>
+      <c r="O117">
+        <v>0.0418351326288</v>
+      </c>
+      <c r="P117">
+        <v>0.08173461940563</v>
+      </c>
+      <c r="Q117">
+        <v>0.1196323344055899</v>
+      </c>
+      <c r="R117">
+        <v>0.1542157510996999</v>
+      </c>
+      <c r="S117">
+        <v>0.183533374712</v>
+      </c>
+      <c r="T117">
+        <v>0.2070388927999999</v>
+      </c>
+    </row>
+    <row r="118" spans="1:20">
+      <c r="A118" t="s">
+        <v>20</v>
+      </c>
+      <c r="B118" t="s">
+        <v>47</v>
+      </c>
+      <c r="C118" t="s">
+        <v>53</v>
+      </c>
+      <c r="D118" t="s">
+        <v>56</v>
+      </c>
+      <c r="E118" t="s">
+        <v>59</v>
+      </c>
+      <c r="H118">
+        <v>1.265134E-07</v>
+      </c>
+      <c r="I118">
+        <v>8.66022E-07</v>
+      </c>
+      <c r="J118">
+        <v>6.0146E-06</v>
+      </c>
+      <c r="K118">
+        <v>6.8088E-06</v>
+      </c>
+      <c r="L118">
+        <v>6.720370000000001E-06</v>
+      </c>
+      <c r="M118">
+        <v>4.98365E-06</v>
+      </c>
+      <c r="N118">
+        <v>3.7962E-06</v>
+      </c>
+      <c r="O118">
+        <v>3.04953E-06</v>
+      </c>
+      <c r="P118">
+        <v>2.52573E-06</v>
+      </c>
+      <c r="Q118">
+        <v>1.143329E-06</v>
+      </c>
+      <c r="R118">
+        <v>5.86145E-07</v>
+      </c>
+      <c r="S118">
+        <v>3.29286E-07</v>
+      </c>
+      <c r="T118">
+        <v>2.002141E-07</v>
+      </c>
+    </row>
+    <row r="119" spans="1:20">
+      <c r="A119" t="s">
+        <v>20</v>
+      </c>
+      <c r="B119" t="s">
+        <v>47</v>
+      </c>
+      <c r="C119" t="s">
+        <v>53</v>
+      </c>
+      <c r="D119" t="s">
+        <v>57</v>
+      </c>
+      <c r="E119" t="s">
+        <v>59</v>
+      </c>
+      <c r="H119">
+        <v>3.04733E-08</v>
+      </c>
+      <c r="I119">
+        <v>5.89793E-07</v>
+      </c>
+      <c r="J119">
+        <v>1.00738E-05</v>
+      </c>
+      <c r="K119">
+        <v>1.2066E-05</v>
+      </c>
+      <c r="L119">
+        <v>1.28442E-05</v>
+      </c>
+      <c r="M119">
+        <v>1.07186E-05</v>
+      </c>
+      <c r="N119">
+        <v>9.186329999999999E-06</v>
+      </c>
+      <c r="O119">
+        <v>8.41898E-06</v>
+      </c>
+      <c r="P119">
+        <v>7.86209E-06</v>
+      </c>
+      <c r="Q119">
+        <v>3.95309E-06</v>
+      </c>
+      <c r="R119">
+        <v>2.15924E-06</v>
+      </c>
+      <c r="S119">
+        <v>1.24707E-06</v>
+      </c>
+      <c r="T119">
+        <v>7.60561E-07</v>
+      </c>
+    </row>
+    <row r="120" spans="1:20">
+      <c r="A120" t="s">
+        <v>20</v>
+      </c>
+      <c r="B120" t="s">
+        <v>48</v>
+      </c>
+      <c r="C120" t="s">
+        <v>53</v>
+      </c>
+      <c r="D120" t="s">
+        <v>56</v>
+      </c>
+      <c r="E120" t="s">
+        <v>59</v>
+      </c>
+      <c r="H120">
+        <v>9.961880000000001E-06</v>
+      </c>
+      <c r="I120">
+        <v>5.02628E-05</v>
+      </c>
+      <c r="J120">
+        <v>0.0002706398</v>
+      </c>
+      <c r="K120">
+        <v>0.0003207034</v>
+      </c>
+      <c r="L120">
+        <v>0.000436372</v>
+      </c>
+      <c r="M120">
+        <v>0.0006344160000000001</v>
+      </c>
+      <c r="N120">
+        <v>0.000995460920272</v>
+      </c>
+      <c r="O120">
+        <v>0.003172450395236</v>
+      </c>
+      <c r="P120">
+        <v>0.00537008709</v>
+      </c>
+      <c r="Q120">
+        <v>0.0014690834209</v>
+      </c>
+      <c r="R120">
+        <v>0.0008962445288020001</v>
+      </c>
+      <c r="S120">
+        <v>0.0005405049999999999</v>
+      </c>
+      <c r="T120">
+        <v>0.000331307</v>
+      </c>
+    </row>
+    <row r="121" spans="1:20">
+      <c r="A121" t="s">
+        <v>20</v>
+      </c>
+      <c r="B121" t="s">
+        <v>48</v>
+      </c>
+      <c r="C121" t="s">
+        <v>53</v>
+      </c>
+      <c r="D121" t="s">
+        <v>57</v>
+      </c>
+      <c r="E121" t="s">
+        <v>59</v>
+      </c>
+      <c r="H121">
+        <v>1.64014E-06</v>
+      </c>
+      <c r="I121">
+        <v>2.1871E-05</v>
+      </c>
+      <c r="J121">
+        <v>0.000314151</v>
+      </c>
+      <c r="K121">
+        <v>0.0004201</v>
+      </c>
+      <c r="L121">
+        <v>0.000605426273644</v>
+      </c>
+      <c r="M121">
+        <v>0.000910623152</v>
+      </c>
+      <c r="N121">
+        <v>0.003467021126263</v>
+      </c>
+      <c r="O121">
+        <v>0.0058060805</v>
+      </c>
+      <c r="P121">
+        <v>0.00905638391087</v>
+      </c>
+      <c r="Q121">
+        <v>0.01079635143</v>
+      </c>
+      <c r="R121">
+        <v>0.0114422886999999</v>
+      </c>
+      <c r="S121">
+        <v>0.001076890538</v>
+      </c>
+      <c r="T121">
+        <v>0.0006016391155640001</v>
+      </c>
+    </row>
+    <row r="122" spans="1:20">
+      <c r="A122" t="s">
+        <v>20</v>
+      </c>
+      <c r="B122" t="s">
+        <v>49</v>
+      </c>
+      <c r="C122" t="s">
+        <v>53</v>
+      </c>
+      <c r="D122" t="s">
+        <v>56</v>
+      </c>
+      <c r="E122" t="s">
+        <v>59</v>
+      </c>
+      <c r="F122">
+        <v>3.13849E-10</v>
+      </c>
+      <c r="G122">
+        <v>1.288821E-09</v>
+      </c>
+      <c r="H122">
+        <v>1.633939E-09</v>
+      </c>
+      <c r="I122">
+        <v>2.287396E-09</v>
+      </c>
+      <c r="J122">
+        <v>3.24291E-09</v>
+      </c>
+      <c r="K122">
+        <v>8.88477E-10</v>
+      </c>
+      <c r="L122">
+        <v>3.30847E-10</v>
+      </c>
+      <c r="M122">
+        <v>1.01778E-10</v>
+      </c>
+    </row>
+    <row r="123" spans="1:20">
+      <c r="A123" t="s">
+        <v>20</v>
+      </c>
+      <c r="B123" t="s">
+        <v>49</v>
+      </c>
+      <c r="C123" t="s">
+        <v>53</v>
+      </c>
+      <c r="D123" t="s">
+        <v>57</v>
+      </c>
+      <c r="E123" t="s">
+        <v>59</v>
+      </c>
+      <c r="G123">
+        <v>1.12107E-10</v>
+      </c>
+      <c r="H123">
+        <v>4.57257E-10</v>
+      </c>
+      <c r="I123">
+        <v>1.87156E-09</v>
+      </c>
+      <c r="J123">
+        <v>7.11763E-09</v>
+      </c>
+      <c r="K123">
+        <v>2.43082E-09</v>
+      </c>
+      <c r="L123">
+        <v>1.07014E-09</v>
+      </c>
+      <c r="M123">
+        <v>5.97593E-10</v>
+      </c>
+      <c r="N123">
+        <v>4.29191E-10</v>
+      </c>
+    </row>
+    <row r="124" spans="1:20">
+      <c r="A124" t="s">
+        <v>20</v>
+      </c>
+      <c r="B124" t="s">
+        <v>50</v>
+      </c>
+      <c r="C124" t="s">
+        <v>53</v>
+      </c>
+      <c r="D124" t="s">
+        <v>56</v>
+      </c>
+      <c r="E124" t="s">
+        <v>59</v>
+      </c>
+      <c r="F124">
+        <v>6.394368999999999E-06</v>
+      </c>
+      <c r="G124">
+        <v>3.795405E-05</v>
+      </c>
+      <c r="H124">
+        <v>0.0001745634</v>
+      </c>
+      <c r="I124">
+        <v>0.001179634</v>
+      </c>
+      <c r="J124">
+        <v>0.0066707</v>
+      </c>
+      <c r="K124">
+        <v>0.00692092</v>
+      </c>
+      <c r="L124">
+        <v>0.009479610845113</v>
+      </c>
+      <c r="M124">
+        <v>0.015711159426924</v>
+      </c>
+      <c r="N124">
+        <v>0.0570369705516299</v>
+      </c>
+      <c r="O124">
+        <v>0.102536104356326</v>
+      </c>
+      <c r="P124">
+        <v>0.19614959773778</v>
+      </c>
+      <c r="Q124">
+        <v>0.27298934245674</v>
+      </c>
+      <c r="R124">
+        <v>0.3446080864069499</v>
+      </c>
+      <c r="S124">
+        <v>0.40622455273473</v>
+      </c>
+      <c r="T124">
+        <v>0.45747359853128</v>
+      </c>
+    </row>
+    <row r="125" spans="1:20">
+      <c r="A125" t="s">
+        <v>20</v>
+      </c>
+      <c r="B125" t="s">
+        <v>50</v>
+      </c>
+      <c r="C125" t="s">
+        <v>53</v>
+      </c>
+      <c r="D125" t="s">
+        <v>57</v>
+      </c>
+      <c r="E125" t="s">
+        <v>59</v>
+      </c>
+      <c r="F125">
+        <v>1.13458E-07</v>
+      </c>
+      <c r="G125">
+        <v>1.89338E-06</v>
+      </c>
+      <c r="H125">
+        <v>2.37906E-05</v>
+      </c>
+      <c r="I125">
+        <v>0.000419155</v>
+      </c>
+      <c r="J125">
+        <v>0.00646741</v>
+      </c>
+      <c r="K125">
+        <v>0.00731253286981</v>
+      </c>
+      <c r="L125">
+        <v>0.010208156476</v>
+      </c>
+      <c r="M125">
+        <v>0.038543812779</v>
+      </c>
+      <c r="N125">
+        <v>0.066256448</v>
+      </c>
+      <c r="O125">
+        <v>0.12242119882</v>
+      </c>
+      <c r="P125">
+        <v>0.244328927539141</v>
+      </c>
+      <c r="Q125">
+        <v>0.361211337624876</v>
+      </c>
+      <c r="R125">
+        <v>0.4669564705319999</v>
+      </c>
+      <c r="S125">
+        <v>0.55392787136</v>
+      </c>
+      <c r="T125">
+        <v>0.6205790148</v>
+      </c>
+    </row>
+    <row r="126" spans="1:20">
+      <c r="A126" t="s">
+        <v>20</v>
+      </c>
+      <c r="B126" t="s">
+        <v>51</v>
+      </c>
+      <c r="C126" t="s">
+        <v>53</v>
+      </c>
+      <c r="D126" t="s">
+        <v>56</v>
+      </c>
+      <c r="E126" t="s">
+        <v>59</v>
+      </c>
+      <c r="H126">
+        <v>5.492722E-07</v>
+      </c>
+      <c r="I126">
+        <v>2.898425E-06</v>
+      </c>
+      <c r="J126">
+        <v>1.995739E-05</v>
+      </c>
+      <c r="K126">
+        <v>2.525045E-05</v>
+      </c>
+      <c r="L126">
+        <v>3.510383E-05</v>
+      </c>
+      <c r="M126">
+        <v>5.151256E-05</v>
+      </c>
+      <c r="N126">
+        <v>7.983931089999999E-05</v>
+      </c>
+      <c r="O126">
+        <v>0.000290137731745</v>
+      </c>
+      <c r="P126">
+        <v>0.0003982664151</v>
+      </c>
+      <c r="Q126">
+        <v>8.291462878E-05</v>
+      </c>
+      <c r="R126">
+        <v>5.21215E-05</v>
+      </c>
+      <c r="S126">
+        <v>3.275935E-05</v>
+      </c>
+      <c r="T126">
+        <v>2.049753E-05</v>
+      </c>
+    </row>
+    <row r="127" spans="1:20">
+      <c r="A127" t="s">
+        <v>20</v>
+      </c>
+      <c r="B127" t="s">
+        <v>51</v>
+      </c>
+      <c r="C127" t="s">
+        <v>53</v>
+      </c>
+      <c r="D127" t="s">
+        <v>57</v>
+      </c>
+      <c r="E127" t="s">
+        <v>59</v>
+      </c>
+      <c r="H127">
+        <v>4.15673E-08</v>
+      </c>
+      <c r="I127">
+        <v>6.81692E-07</v>
+      </c>
+      <c r="J127">
+        <v>1.36358E-05</v>
+      </c>
+      <c r="K127">
+        <v>1.80832E-05</v>
+      </c>
+      <c r="L127">
+        <v>2.66353E-05</v>
+      </c>
+      <c r="M127">
+        <v>4.13955E-05</v>
+      </c>
+      <c r="N127">
+        <v>0.00015623245</v>
+      </c>
+      <c r="O127">
+        <v>0.00026115539</v>
+      </c>
+      <c r="P127">
+        <v>0.000408666084</v>
+      </c>
+      <c r="Q127">
+        <v>0.00049626703</v>
+      </c>
+      <c r="R127">
+        <v>0.0005391015</v>
+      </c>
+      <c r="S127">
+        <v>5.5776244275E-05</v>
+      </c>
+      <c r="T127">
+        <v>3.8314E-05</v>
+      </c>
+    </row>
+    <row r="128" spans="1:20">
+      <c r="A128" t="s">
+        <v>20</v>
+      </c>
+      <c r="B128" t="s">
+        <v>52</v>
+      </c>
+      <c r="C128" t="s">
+        <v>53</v>
+      </c>
+      <c r="D128" t="s">
+        <v>56</v>
+      </c>
+      <c r="E128" t="s">
+        <v>59</v>
+      </c>
+      <c r="F128">
+        <v>1.6757862585E-05</v>
+      </c>
+      <c r="G128">
+        <v>8.6421129421E-05</v>
+      </c>
+      <c r="H128">
+        <v>0.000602339942839</v>
+      </c>
+      <c r="I128">
+        <v>0.004044247840396</v>
+      </c>
+      <c r="J128">
+        <v>0.02489174829291</v>
+      </c>
+      <c r="K128">
+        <v>0.0301833939727839</v>
+      </c>
+      <c r="L128">
+        <v>0.0425536682300019</v>
+      </c>
+      <c r="M128">
+        <v>0.0739406904199217</v>
+      </c>
+      <c r="N128">
+        <v>0.1899678699466419</v>
+      </c>
+      <c r="O128">
+        <v>0.3960981813274686</v>
+      </c>
+      <c r="P128">
+        <v>0.7751281787606785</v>
+      </c>
+      <c r="Q128">
+        <v>1.091522607484418</v>
+      </c>
+      <c r="R128">
+        <v>1.395016425007189</v>
+      </c>
+      <c r="S128">
+        <v>1.644699567622053</v>
+      </c>
+      <c r="T128">
+        <v>1.860986417180167</v>
+      </c>
+    </row>
+    <row r="129" spans="1:20">
+      <c r="A129" t="s">
+        <v>20</v>
+      </c>
+      <c r="B129" t="s">
+        <v>52</v>
+      </c>
+      <c r="C129" t="s">
+        <v>53</v>
+      </c>
+      <c r="D129" t="s">
+        <v>57</v>
+      </c>
+      <c r="E129" t="s">
+        <v>59</v>
+      </c>
+      <c r="F129">
+        <v>2.81987333E-07</v>
+      </c>
+      <c r="G129">
+        <v>4.376287237E-06</v>
+      </c>
+      <c r="H129">
+        <v>9.2618067657E-05</v>
+      </c>
+      <c r="I129">
+        <v>0.00157615963456</v>
+      </c>
+      <c r="J129">
+        <v>0.02487944599763</v>
+      </c>
+      <c r="K129">
+        <v>0.03469332930076</v>
+      </c>
+      <c r="L129">
+        <v>0.06514327404816379</v>
+      </c>
+      <c r="M129">
+        <v>0.152932417455341</v>
+      </c>
+      <c r="N129">
+        <v>0.2673057486830559</v>
+      </c>
+      <c r="O129">
+        <v>0.489642485398314</v>
+      </c>
+      <c r="P129">
+        <v>0.9653195916744858</v>
+      </c>
+      <c r="Q129">
+        <v>1.413910652280567</v>
+      </c>
+      <c r="R129">
+        <v>1.818953656409839</v>
+      </c>
+      <c r="S129">
+        <v>2.142135248170485</v>
+      </c>
+      <c r="T129">
+        <v>2.400616294946764</v>
       </c>
     </row>
   </sheetData>

</xml_diff>